<commit_message>
Applied Fudge Factor System Not Particularly Well, But Got Localization to 1/10th of An Inch
</commit_message>
<xml_diff>
--- a/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
+++ b/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/Dropbox/Brain Stormz FTC/2023-24-code/AprilTag Performance Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532336B7-B56D-4248-8A5F-0A5D717EE073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD8F713-5EC1-AE42-B84F-E392BEF0F02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
   <si>
     <t>Point</t>
   </si>
@@ -216,17 +216,42 @@
     <t>Delta Y</t>
   </si>
   <si>
-    <t>Delta H</t>
+    <t>Fudge factor?</t>
+  </si>
+  <si>
+    <t>realistic error: sub 0.5</t>
+  </si>
+  <si>
+    <t>Delta H (deg)</t>
+  </si>
+  <si>
+    <t>Delta Y - fudge</t>
+  </si>
+  <si>
+    <t>ID4 visible, sheared to the right… in the center of image. Bad.</t>
+  </si>
+  <si>
+    <t>delta X - fudge</t>
+  </si>
+  <si>
+    <t>delta H - fudge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -258,8 +283,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -873,10 +899,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC64249A-AA8D-F049-BD4E-E239A34687E9}">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="157" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -886,6 +912,8 @@
     <col min="8" max="8" width="28" customWidth="1"/>
     <col min="9" max="9" width="25.83203125" customWidth="1"/>
     <col min="10" max="10" width="19.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.5" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
@@ -926,7 +954,7 @@
         <v>58</v>
       </c>
       <c r="N1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="Q1" t="s">
         <v>9</v>
@@ -1029,7 +1057,7 @@
         <v>-6.6999999999999886</v>
       </c>
       <c r="Q3" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -1220,7 +1248,7 @@
         <f t="shared" si="1"/>
         <v>0.60000000000000142</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="2">
         <f t="shared" si="0"/>
         <v>3.2000000000000028</v>
       </c>
@@ -1330,6 +1358,9 @@
         <f>180+13</f>
         <v>193</v>
       </c>
+      <c r="M10" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1354,7 +1385,120 @@
         <v>182</v>
       </c>
     </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L12">
+        <f>AVERAGE(L2, L4:L8)</f>
+        <v>0.4666666666666674</v>
+      </c>
+      <c r="M12">
+        <f t="shared" ref="M12:N12" si="3">AVERAGE(M2, M4:M8)</f>
+        <v>2.5833333333333335</v>
+      </c>
+      <c r="N12">
+        <f>AVERAGE(N2, N4:N8)</f>
+        <v>6.2166666666666641</v>
+      </c>
+      <c r="P12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L14" t="s">
+        <v>64</v>
+      </c>
+      <c r="M14" t="s">
+        <v>62</v>
+      </c>
+      <c r="N14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L15">
+        <f>L2 - $L$12</f>
+        <v>0.13333333333333403</v>
+      </c>
+      <c r="M15">
+        <f>2.4 - M12</f>
+        <v>-0.18333333333333357</v>
+      </c>
+      <c r="N15">
+        <f>N2 - $N$12</f>
+        <v>2.6833333333333416</v>
+      </c>
+    </row>
+    <row r="17" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <f t="shared" ref="L16:N21" si="4">L4 - $L$12</f>
+        <v>3.3333333333332604E-2</v>
+      </c>
+      <c r="M17">
+        <f>2.3 -M12</f>
+        <v>-0.28333333333333366</v>
+      </c>
+      <c r="N17">
+        <f t="shared" ref="N16:N21" si="5">N4 - $N$12</f>
+        <v>-1.6666666666675489E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L18">
+        <f t="shared" si="4"/>
+        <v>0.18333333333333118</v>
+      </c>
+      <c r="M18">
+        <f>2.4-M12</f>
+        <v>-0.18333333333333357</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="5"/>
+        <v>1.7833333333333359</v>
+      </c>
+    </row>
+    <row r="19" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L19">
+        <f>L6 - $L$12</f>
+        <v>-0.36666666666666597</v>
+      </c>
+      <c r="M19">
+        <f>2.7-M12</f>
+        <v>0.1166666666666667</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="5"/>
+        <v>-0.21666666666666412</v>
+      </c>
+    </row>
+    <row r="20" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L20">
+        <f t="shared" si="4"/>
+        <v>0.13333333333333403</v>
+      </c>
+      <c r="M20">
+        <f>3.2 - M12</f>
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="5"/>
+        <v>-3.5166666666666755</v>
+      </c>
+    </row>
+    <row r="21" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L21">
+        <f t="shared" si="4"/>
+        <v>-0.11666666666666597</v>
+      </c>
+      <c r="M21">
+        <f>2.5 - M12</f>
+        <v>-8.3333333333333481E-2</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="5"/>
+        <v>-0.71666666666666412</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Working Offset From The Past, Proof that ids 4, 5, 6 are reliable to 1 inch from basically anywhere
</commit_message>
<xml_diff>
--- a/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
+++ b/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/Dropbox/Brain Stormz FTC/2023-24-code/AprilTag Performance Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD8F713-5EC1-AE42-B84F-E392BEF0F02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF8A3E3-BA1E-F44D-A360-315012DE6214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="89">
   <si>
     <t>Point</t>
   </si>
@@ -235,13 +238,82 @@
   </si>
   <si>
     <t>delta H - fudge</t>
+  </si>
+  <si>
+    <t>NEW FUDGE FACTOR CALCULATOR</t>
+  </si>
+  <si>
+    <t>FudgeY:</t>
+  </si>
+  <si>
+    <t>FudgeX:</t>
+  </si>
+  <si>
+    <t>FudgeYNew:</t>
+  </si>
+  <si>
+    <t>FudgeXNew:</t>
+  </si>
+  <si>
+    <t>COORD</t>
+  </si>
+  <si>
+    <t>(0, 1)</t>
+  </si>
+  <si>
+    <t>(0, 2)</t>
+  </si>
+  <si>
+    <t>(0, 3)</t>
+  </si>
+  <si>
+    <t>(1, 1)</t>
+  </si>
+  <si>
+    <t>(1, 2)</t>
+  </si>
+  <si>
+    <t>(1, 3)</t>
+  </si>
+  <si>
+    <t>(2, 1)</t>
+  </si>
+  <si>
+    <t>(2, 2)</t>
+  </si>
+  <si>
+    <t>(2, 3)</t>
+  </si>
+  <si>
+    <t>(3, 1)</t>
+  </si>
+  <si>
+    <t>(3, 2)</t>
+  </si>
+  <si>
+    <t>(3, 3)</t>
+  </si>
+  <si>
+    <t>(5, 2)</t>
+  </si>
+  <si>
+    <t>(-4B)</t>
+  </si>
+  <si>
+    <t>(3, 0)</t>
+  </si>
+  <si>
+    <t>(2, 0)</t>
+  </si>
+  <si>
+    <t>(1,0)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -261,6 +333,12 @@
       <color rgb="FF000000"/>
       <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF2AACB8"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -283,10 +361,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,7 +708,7 @@
       <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" customWidth="1"/>
@@ -635,7 +716,7 @@
     <col min="6" max="6" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -664,7 +745,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -693,7 +774,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -722,7 +803,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -751,7 +832,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -762,7 +843,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -791,7 +872,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -820,7 +901,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -828,7 +909,7 @@
         <v>27.25</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -836,7 +917,7 @@
         <v>34.375</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -844,7 +925,7 @@
         <v>41.625</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -852,7 +933,7 @@
         <v>26.875</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -860,7 +941,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -868,7 +949,7 @@
         <v>41.5</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -876,7 +957,7 @@
         <v>26.5625</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -884,7 +965,7 @@
         <v>33.75</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -901,11 +982,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC64249A-AA8D-F049-BD4E-E239A34687E9}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="5" max="5" width="20.33203125" customWidth="1"/>
@@ -916,7 +997,7 @@
     <col min="13" max="13" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -960,7 +1041,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1010,7 +1091,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1060,7 +1141,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1095,7 +1176,7 @@
         <v>238</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L11" si="1" xml:space="preserve"> F4 - ABS(C4)</f>
+        <f t="shared" ref="L4:L8" si="1" xml:space="preserve"> F4 - ABS(C4)</f>
         <v>0.5</v>
       </c>
       <c r="M4">
@@ -1110,7 +1191,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1160,7 +1241,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1203,14 +1284,14 @@
         <v>2.7000000000000028</v>
       </c>
       <c r="N6">
-        <f t="shared" ref="N3:N8" si="2" xml:space="preserve"> H6 - ABS(E6)</f>
+        <f t="shared" ref="N6" si="2" xml:space="preserve"> H6 - ABS(E6)</f>
         <v>6</v>
       </c>
       <c r="Q6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -1260,7 +1341,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -1310,7 +1391,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -1336,7 +1417,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1362,7 +1443,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1385,13 +1466,13 @@
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17">
       <c r="L12">
         <f>AVERAGE(L2, L4:L8)</f>
         <v>0.4666666666666674</v>
       </c>
       <c r="M12">
-        <f t="shared" ref="M12:N12" si="3">AVERAGE(M2, M4:M8)</f>
+        <f t="shared" ref="M12" si="3">AVERAGE(M2, M4:M8)</f>
         <v>2.5833333333333335</v>
       </c>
       <c r="N12">
@@ -1402,7 +1483,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17">
       <c r="L14" t="s">
         <v>64</v>
       </c>
@@ -1413,7 +1494,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17">
       <c r="L15">
         <f>L2 - $L$12</f>
         <v>0.13333333333333403</v>
@@ -1427,9 +1508,9 @@
         <v>2.6833333333333416</v>
       </c>
     </row>
-    <row r="17" spans="12:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="12:14">
       <c r="L17">
-        <f t="shared" ref="L16:N21" si="4">L4 - $L$12</f>
+        <f t="shared" ref="L17:L21" si="4">L4 - $L$12</f>
         <v>3.3333333333332604E-2</v>
       </c>
       <c r="M17">
@@ -1437,11 +1518,11 @@
         <v>-0.28333333333333366</v>
       </c>
       <c r="N17">
-        <f t="shared" ref="N16:N21" si="5">N4 - $N$12</f>
+        <f t="shared" ref="N17:N21" si="5">N4 - $N$12</f>
         <v>-1.6666666666675489E-2</v>
       </c>
     </row>
-    <row r="18" spans="12:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="12:14">
       <c r="L18">
         <f t="shared" si="4"/>
         <v>0.18333333333333118</v>
@@ -1455,7 +1536,7 @@
         <v>1.7833333333333359</v>
       </c>
     </row>
-    <row r="19" spans="12:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="12:14">
       <c r="L19">
         <f>L6 - $L$12</f>
         <v>-0.36666666666666597</v>
@@ -1469,7 +1550,7 @@
         <v>-0.21666666666666412</v>
       </c>
     </row>
-    <row r="20" spans="12:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="12:14">
       <c r="L20">
         <f t="shared" si="4"/>
         <v>0.13333333333333403</v>
@@ -1483,7 +1564,7 @@
         <v>-3.5166666666666755</v>
       </c>
     </row>
-    <row r="21" spans="12:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="12:14">
       <c r="L21">
         <f t="shared" si="4"/>
         <v>-0.11666666666666597</v>
@@ -1501,4 +1582,2211 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA783638-C337-8141-A9ED-555EF0FD6A27}">
+  <dimension ref="B1:Q49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:T50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="8" max="8" width="28" customWidth="1"/>
+    <col min="9" max="9" width="25.83203125" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.5" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:17">
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="2:17">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1">
+        <v>-41.9</v>
+      </c>
+      <c r="D2" s="1">
+        <v>-37.6</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2">
+        <v>41.25</v>
+      </c>
+      <c r="G2">
+        <v>38</v>
+      </c>
+      <c r="L2">
+        <f xml:space="preserve"> F2 - ABS(C2)</f>
+        <v>-0.64999999999999858</v>
+      </c>
+      <c r="M2">
+        <f xml:space="preserve"> G2 - ABS(D2)</f>
+        <v>0.39999999999999858</v>
+      </c>
+      <c r="N2">
+        <f xml:space="preserve"> H2 - ABS(E2)</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1">
+        <v>-35.5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-37.4</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3">
+        <v>35.5</v>
+      </c>
+      <c r="G3">
+        <v>38</v>
+      </c>
+      <c r="L3">
+        <f xml:space="preserve"> F3 - ABS(C3)</f>
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:N8" si="0" xml:space="preserve"> G3 - ABS(D3)</f>
+        <v>0.60000000000000142</v>
+      </c>
+      <c r="N3">
+        <f>H3 - ABS(E3)</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17">
+      <c r="C4" s="1">
+        <v>-28.9</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-37.4</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4">
+        <v>28.5</v>
+      </c>
+      <c r="G4">
+        <v>38</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L8" si="1" xml:space="preserve"> F4 - ABS(C4)</f>
+        <v>-0.39999999999999858</v>
+      </c>
+      <c r="M4">
+        <f xml:space="preserve"> G4 - ABS(D4)</f>
+        <v>0.60000000000000142</v>
+      </c>
+      <c r="N4">
+        <f xml:space="preserve"> I4 - E4</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17">
+      <c r="C5" s="1">
+        <v>-29.1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-47.6</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5">
+        <v>28.5</v>
+      </c>
+      <c r="G5">
+        <v>48</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>-0.60000000000000142</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>0.39999999999999858</v>
+      </c>
+      <c r="N5">
+        <f xml:space="preserve"> J5 - ABS(E5)</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17">
+      <c r="C6" s="1">
+        <v>-35.700000000000003</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-47.7</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6">
+        <v>35.5</v>
+      </c>
+      <c r="G6">
+        <v>48</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>-0.20000000000000284</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>0.29999999999999716</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17">
+      <c r="C7" s="1">
+        <v>-41.5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>-47.8</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7">
+        <v>41.25</v>
+      </c>
+      <c r="G7">
+        <v>48</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>-0.25</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.20000000000000284</v>
+      </c>
+      <c r="N7">
+        <f xml:space="preserve"> I7 - ABS(E7)</f>
+        <v>0</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1">
+        <v>-28.5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>-56.7</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8">
+        <v>28.5</v>
+      </c>
+      <c r="G8">
+        <v>57</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>0.29999999999999716</v>
+      </c>
+      <c r="N8">
+        <f xml:space="preserve"> J8 - ABS(E8)</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17">
+      <c r="C9" s="1">
+        <v>-35.4</v>
+      </c>
+      <c r="D9" s="1">
+        <v>-56.9</v>
+      </c>
+      <c r="F9">
+        <v>35.5</v>
+      </c>
+      <c r="G9">
+        <v>57</v>
+      </c>
+      <c r="L9">
+        <f xml:space="preserve"> F9 - ABS(C9)</f>
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="M9">
+        <f xml:space="preserve"> G9 - ABS(D9)</f>
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="N9">
+        <f xml:space="preserve"> H9 - ABS(E9)</f>
+        <v>0</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17">
+      <c r="C10" s="1">
+        <v>-41.1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>-56.9</v>
+      </c>
+      <c r="F10">
+        <v>41.25</v>
+      </c>
+      <c r="G10">
+        <v>57</v>
+      </c>
+      <c r="L10">
+        <f xml:space="preserve"> F10 - ABS(C10)</f>
+        <v>0.14999999999999858</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ref="M10" si="2" xml:space="preserve"> G10 - ABS(D10)</f>
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="N10">
+        <f>H10 - ABS(E10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17">
+      <c r="C11" s="1">
+        <v>-35.5</v>
+      </c>
+      <c r="D11" s="1">
+        <v>-37.6</v>
+      </c>
+      <c r="F11">
+        <v>35.5</v>
+      </c>
+      <c r="G11">
+        <v>38</v>
+      </c>
+      <c r="L11">
+        <f t="shared" ref="L11:L12" si="3" xml:space="preserve"> F11 - ABS(C11)</f>
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <f xml:space="preserve"> G11 - ABS(D11)</f>
+        <v>0.39999999999999858</v>
+      </c>
+      <c r="N11">
+        <f t="shared" ref="N11:N13" si="4">H11 - ABS(E11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17">
+      <c r="C12" s="1">
+        <v>-29.3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-37.299999999999997</v>
+      </c>
+      <c r="F12">
+        <v>28.5</v>
+      </c>
+      <c r="G12">
+        <v>38</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="3"/>
+        <v>-0.80000000000000071</v>
+      </c>
+      <c r="M12">
+        <f t="shared" ref="M12:M13" si="5" xml:space="preserve"> G12 - ABS(D12)</f>
+        <v>0.70000000000000284</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17">
+      <c r="C13" s="1">
+        <v>-29.3</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-37.4</v>
+      </c>
+      <c r="F13">
+        <v>28.5</v>
+      </c>
+      <c r="G13">
+        <v>38</v>
+      </c>
+      <c r="L13">
+        <f xml:space="preserve"> F13 - ABS(C13)</f>
+        <v>-0.80000000000000071</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="5"/>
+        <v>0.60000000000000142</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17">
+      <c r="C14" s="1">
+        <v>-29.1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-35.1</v>
+      </c>
+      <c r="F14">
+        <v>28.5</v>
+      </c>
+      <c r="G14">
+        <v>36</v>
+      </c>
+      <c r="L14">
+        <f xml:space="preserve"> F14 - ABS(C14)</f>
+        <v>-0.60000000000000142</v>
+      </c>
+      <c r="M14">
+        <f xml:space="preserve"> G14 - ABS(D14)</f>
+        <v>0.89999999999999858</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17">
+      <c r="C15" s="1">
+        <v>-20.5</v>
+      </c>
+      <c r="D15" s="1">
+        <v>-37.299999999999997</v>
+      </c>
+      <c r="F15">
+        <v>20.125</v>
+      </c>
+      <c r="G15">
+        <v>37.875</v>
+      </c>
+      <c r="L15">
+        <f>F15 - ABS( C15)</f>
+        <v>-0.375</v>
+      </c>
+      <c r="M15">
+        <f>G15 - ABS(D15)</f>
+        <v>0.57500000000000284</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17">
+      <c r="C16" s="1">
+        <v>-44.2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>-35.9</v>
+      </c>
+    </row>
+    <row r="19" spans="12:14">
+      <c r="M19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="12:14">
+      <c r="L21">
+        <f>AVERAGE(L2:L10, L11:L15)</f>
+        <v>-0.31607142857142889</v>
+      </c>
+      <c r="M21">
+        <f>AVERAGE(M2:M10)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="N21">
+        <f>AVERAGE(N2, N4:N8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="12:14">
+      <c r="L23" t="s">
+        <v>64</v>
+      </c>
+      <c r="M23" t="s">
+        <v>62</v>
+      </c>
+      <c r="N23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="12:14">
+      <c r="L24">
+        <f>L2 - $L$21</f>
+        <v>-0.33392857142856969</v>
+      </c>
+      <c r="M24">
+        <f>M2 - $M$21</f>
+        <v>6.6666666666665264E-2</v>
+      </c>
+      <c r="N24">
+        <f>N2 - $N$21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="12:14">
+      <c r="L25">
+        <f>L3 - $L$21</f>
+        <v>0.31607142857142889</v>
+      </c>
+      <c r="M25">
+        <f t="shared" ref="M25:M40" si="6">M3 - $M$21</f>
+        <v>0.26666666666666811</v>
+      </c>
+      <c r="N25">
+        <f t="shared" ref="N25:N30" si="7">N3 - $N$21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="12:14">
+      <c r="L26">
+        <f>L4 - $L$21</f>
+        <v>-8.3928571428569687E-2</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="6"/>
+        <v>0.26666666666666811</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="12:14">
+      <c r="L27">
+        <f>L5 - $L$21</f>
+        <v>-0.28392857142857253</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="6"/>
+        <v>6.6666666666665264E-2</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="12:14">
+      <c r="L28">
+        <f>L6 - $L$21</f>
+        <v>0.11607142857142605</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="6"/>
+        <v>-3.3333333333336157E-2</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="12:14">
+      <c r="L29">
+        <f>L7 - $L$21</f>
+        <v>6.6071428571428892E-2</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="6"/>
+        <v>-0.13333333333333047</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="12:14">
+      <c r="L30">
+        <f>L8 - $L$21</f>
+        <v>0.31607142857142889</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="6"/>
+        <v>-3.3333333333336157E-2</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="12:14">
+      <c r="L31">
+        <f>L9 - $L$21</f>
+        <v>0.41607142857143031</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="6"/>
+        <v>-0.23333333333333189</v>
+      </c>
+    </row>
+    <row r="32" spans="12:14">
+      <c r="L32">
+        <f>L10 - $L$21</f>
+        <v>0.46607142857142747</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="6"/>
+        <v>-0.23333333333333189</v>
+      </c>
+    </row>
+    <row r="34" spans="12:13">
+      <c r="L34">
+        <f>L11 - $L$21</f>
+        <v>0.31607142857142889</v>
+      </c>
+      <c r="M34">
+        <f>M11 - $M$21</f>
+        <v>6.6666666666665264E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="12:13">
+      <c r="L35">
+        <f>L12 - $L$21</f>
+        <v>-0.48392857142857182</v>
+      </c>
+      <c r="M35">
+        <f>M12 - $M$21</f>
+        <v>0.36666666666666953</v>
+      </c>
+    </row>
+    <row r="36" spans="12:13">
+      <c r="L36">
+        <f>L13 - $L$21</f>
+        <v>-0.48392857142857182</v>
+      </c>
+      <c r="M36">
+        <f>M13 - $M$21</f>
+        <v>0.26666666666666811</v>
+      </c>
+    </row>
+    <row r="37" spans="12:13">
+      <c r="L37">
+        <f>L14 - $L$21</f>
+        <v>-0.28392857142857253</v>
+      </c>
+      <c r="M37">
+        <f>M14 - $M$21</f>
+        <v>0.56666666666666532</v>
+      </c>
+    </row>
+    <row r="38" spans="12:13">
+      <c r="L38">
+        <f>L15 - $L$21</f>
+        <v>-5.8928571428571108E-2</v>
+      </c>
+      <c r="M38">
+        <f>M15 - $M$21</f>
+        <v>0.24166666666666953</v>
+      </c>
+    </row>
+    <row r="39" spans="12:13">
+      <c r="L39">
+        <f>L17 - $L$21</f>
+        <v>0.31607142857142889</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="6"/>
+        <v>-0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="40" spans="12:13">
+      <c r="L40">
+        <f>L18 - $L$21</f>
+        <v>0.31607142857142889</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="6"/>
+        <v>-0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="43" spans="12:13">
+      <c r="L43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="12:13">
+      <c r="L45" t="s">
+        <v>67</v>
+      </c>
+      <c r="M45" s="3">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="46" spans="12:13">
+      <c r="L46" t="s">
+        <v>68</v>
+      </c>
+      <c r="M46" s="3">
+        <v>2.58</v>
+      </c>
+    </row>
+    <row r="48" spans="12:13">
+      <c r="L48" t="s">
+        <v>69</v>
+      </c>
+      <c r="M48">
+        <f>M45+M21</f>
+        <v>0.80333333333333323</v>
+      </c>
+    </row>
+    <row r="49" spans="12:13">
+      <c r="L49" t="s">
+        <v>70</v>
+      </c>
+      <c r="M49">
+        <f>M46+M21</f>
+        <v>2.9133333333333336</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DAAFFAD-0131-5640-936C-907E0411A2F0}">
+  <dimension ref="B1:Q69"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="2:17">
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="2:17">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1">
+        <v>-41.9</v>
+      </c>
+      <c r="D2" s="1">
+        <v>-37.6</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2">
+        <v>41.25</v>
+      </c>
+      <c r="G2">
+        <v>38</v>
+      </c>
+      <c r="L2">
+        <f xml:space="preserve"> F2 - ABS(C2)</f>
+        <v>-0.64999999999999858</v>
+      </c>
+      <c r="M2">
+        <f xml:space="preserve"> G2 - ABS(D2)</f>
+        <v>0.39999999999999858</v>
+      </c>
+      <c r="N2">
+        <f xml:space="preserve"> H2 - ABS(E2)</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1">
+        <v>-35.5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-37.4</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3">
+        <v>35.5</v>
+      </c>
+      <c r="G3">
+        <v>38</v>
+      </c>
+      <c r="L3">
+        <f xml:space="preserve"> F3 - ABS(C3)</f>
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:N8" si="0" xml:space="preserve"> G3 - ABS(D3)</f>
+        <v>0.60000000000000142</v>
+      </c>
+      <c r="N3">
+        <f>H3 - ABS(E3)</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17">
+      <c r="C4" s="1">
+        <v>-28.9</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-37.4</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4">
+        <v>28.5</v>
+      </c>
+      <c r="G4">
+        <v>38</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L8" si="1" xml:space="preserve"> F4 - ABS(C4)</f>
+        <v>-0.39999999999999858</v>
+      </c>
+      <c r="M4">
+        <f xml:space="preserve"> G4 - ABS(D4)</f>
+        <v>0.60000000000000142</v>
+      </c>
+      <c r="N4">
+        <f xml:space="preserve"> I4 - E4</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17">
+      <c r="C5" s="1">
+        <v>-29.1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-47.6</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5">
+        <v>28.5</v>
+      </c>
+      <c r="G5">
+        <v>48</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>-0.60000000000000142</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>0.39999999999999858</v>
+      </c>
+      <c r="N5">
+        <f xml:space="preserve"> J5 - ABS(E5)</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17">
+      <c r="C6" s="1">
+        <v>-35.700000000000003</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-47.7</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6">
+        <v>35.5</v>
+      </c>
+      <c r="G6">
+        <v>48</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>-0.20000000000000284</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>0.29999999999999716</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17">
+      <c r="C7" s="1">
+        <v>-41.5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>-47.8</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7">
+        <v>41.25</v>
+      </c>
+      <c r="G7">
+        <v>48</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>-0.25</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.20000000000000284</v>
+      </c>
+      <c r="N7">
+        <f xml:space="preserve"> I7 - ABS(E7)</f>
+        <v>0</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1">
+        <v>-28.5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>-56.7</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8">
+        <v>28.5</v>
+      </c>
+      <c r="G8">
+        <v>57</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>0.29999999999999716</v>
+      </c>
+      <c r="N8">
+        <f xml:space="preserve"> J8 - ABS(E8)</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17">
+      <c r="C9" s="1">
+        <v>-35.4</v>
+      </c>
+      <c r="D9" s="1">
+        <v>-56.9</v>
+      </c>
+      <c r="F9">
+        <v>35.5</v>
+      </c>
+      <c r="G9">
+        <v>57</v>
+      </c>
+      <c r="L9">
+        <f xml:space="preserve"> F9 - ABS(C9)</f>
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="M9">
+        <f xml:space="preserve"> G9 - ABS(D9)</f>
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="N9">
+        <f xml:space="preserve"> H9 - ABS(E9)</f>
+        <v>0</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17">
+      <c r="C10" s="1">
+        <v>-41.1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>-56.9</v>
+      </c>
+      <c r="F10">
+        <v>41.25</v>
+      </c>
+      <c r="G10">
+        <v>57</v>
+      </c>
+      <c r="L10">
+        <f xml:space="preserve"> F10 - ABS(C10)</f>
+        <v>0.14999999999999858</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ref="M10" si="2" xml:space="preserve"> G10 - ABS(D10)</f>
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="N10">
+        <f>H10 - ABS(E10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17">
+      <c r="C11" s="1">
+        <v>-35.5</v>
+      </c>
+      <c r="D11" s="1">
+        <v>-37.6</v>
+      </c>
+      <c r="F11">
+        <v>35.5</v>
+      </c>
+      <c r="G11">
+        <v>38</v>
+      </c>
+      <c r="L11">
+        <f t="shared" ref="L11:M13" si="3" xml:space="preserve"> F11 - ABS(C11)</f>
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <f xml:space="preserve"> G11 - ABS(D11)</f>
+        <v>0.39999999999999858</v>
+      </c>
+      <c r="N11">
+        <f t="shared" ref="N11:N13" si="4">H11 - ABS(E11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17">
+      <c r="C12" s="1">
+        <v>-29.3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-37.299999999999997</v>
+      </c>
+      <c r="F12">
+        <v>28.5</v>
+      </c>
+      <c r="G12">
+        <v>38</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="3"/>
+        <v>-0.80000000000000071</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="3"/>
+        <v>0.70000000000000284</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17">
+      <c r="C13" s="1">
+        <v>-29.3</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-37.4</v>
+      </c>
+      <c r="F13">
+        <v>28.5</v>
+      </c>
+      <c r="G13">
+        <v>38</v>
+      </c>
+      <c r="L13">
+        <f xml:space="preserve"> F13 - ABS(C13)</f>
+        <v>-0.80000000000000071</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="3"/>
+        <v>0.60000000000000142</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17">
+      <c r="C14" s="1">
+        <v>-29.1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-35.1</v>
+      </c>
+      <c r="F14">
+        <v>28.5</v>
+      </c>
+      <c r="G14">
+        <v>36</v>
+      </c>
+      <c r="L14">
+        <f xml:space="preserve"> F14 - ABS(C14)</f>
+        <v>-0.60000000000000142</v>
+      </c>
+      <c r="M14">
+        <f xml:space="preserve"> G14 - ABS(D14)</f>
+        <v>0.89999999999999858</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17">
+      <c r="C15" s="1">
+        <v>-20.5</v>
+      </c>
+      <c r="D15" s="1">
+        <v>-37.299999999999997</v>
+      </c>
+      <c r="F15">
+        <v>20.125</v>
+      </c>
+      <c r="G15">
+        <v>37.875</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17">
+      <c r="C16" s="1">
+        <v>-44.2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>-35.9</v>
+      </c>
+    </row>
+    <row r="19" spans="3:14">
+      <c r="C19" s="1">
+        <v>-43.7</v>
+      </c>
+      <c r="F19">
+        <v>41.25</v>
+      </c>
+    </row>
+    <row r="20" spans="3:14">
+      <c r="C20" s="1">
+        <v>-36</v>
+      </c>
+      <c r="F20">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="3:14">
+      <c r="C22" s="1">
+        <v>-40.5</v>
+      </c>
+      <c r="D22" s="1">
+        <v>-54.3</v>
+      </c>
+      <c r="F22">
+        <v>41.25</v>
+      </c>
+      <c r="G22">
+        <v>57</v>
+      </c>
+      <c r="L22">
+        <f xml:space="preserve"> F22 - ABS(C22)</f>
+        <v>0.75</v>
+      </c>
+      <c r="M22">
+        <f xml:space="preserve"> G22 - ABS(D22)</f>
+        <v>2.7000000000000028</v>
+      </c>
+      <c r="N22">
+        <f t="shared" ref="N22:N33" si="5">H22 - ABS(E22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:14">
+      <c r="C23" s="1">
+        <v>-41.2</v>
+      </c>
+      <c r="D23" s="1">
+        <v>-47.8</v>
+      </c>
+      <c r="F23" s="1">
+        <v>41.25</v>
+      </c>
+      <c r="G23">
+        <v>48</v>
+      </c>
+      <c r="L23">
+        <f xml:space="preserve"> F23 - ABS(C23)</f>
+        <v>4.9999999999997158E-2</v>
+      </c>
+      <c r="M23">
+        <f t="shared" ref="M22:M33" si="6" xml:space="preserve"> G23 - ABS(D23)</f>
+        <v>0.20000000000000284</v>
+      </c>
+    </row>
+    <row r="24" spans="3:14">
+      <c r="C24" s="1">
+        <v>-41</v>
+      </c>
+      <c r="D24" s="1">
+        <v>-56.9</v>
+      </c>
+      <c r="F24">
+        <v>41.25</v>
+      </c>
+      <c r="G24">
+        <v>57</v>
+      </c>
+      <c r="L24">
+        <f xml:space="preserve"> F24 - ABS(C24)</f>
+        <v>0.25</v>
+      </c>
+      <c r="M24">
+        <f xml:space="preserve"> G24 - ABS(D24)</f>
+        <v>0.10000000000000142</v>
+      </c>
+    </row>
+    <row r="25" spans="3:14">
+      <c r="C25" s="1">
+        <v>-35.4</v>
+      </c>
+      <c r="D25" s="1">
+        <v>-56.9</v>
+      </c>
+      <c r="F25">
+        <v>35.5</v>
+      </c>
+      <c r="G25">
+        <v>57</v>
+      </c>
+      <c r="L25">
+        <f xml:space="preserve"> F25 - ABS(C25)</f>
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="M25">
+        <f t="shared" ref="M25:M33" si="7" xml:space="preserve"> G25 - ABS(D25)</f>
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="N25">
+        <f t="shared" ref="N25:N33" si="8">H25 - ABS(E25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="3:14">
+      <c r="C26" s="1">
+        <v>-28.5</v>
+      </c>
+      <c r="D26" s="1">
+        <v>-56.7</v>
+      </c>
+      <c r="F26">
+        <v>28.5</v>
+      </c>
+      <c r="G26">
+        <v>57</v>
+      </c>
+      <c r="L26">
+        <f xml:space="preserve"> F26 - ABS(C26)</f>
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="7"/>
+        <v>0.29999999999999716</v>
+      </c>
+    </row>
+    <row r="27" spans="3:14">
+      <c r="C27" s="1">
+        <v>-28.8</v>
+      </c>
+      <c r="D27" s="4">
+        <v>-47.6</v>
+      </c>
+      <c r="F27">
+        <v>28.5</v>
+      </c>
+      <c r="G27">
+        <v>48</v>
+      </c>
+      <c r="L27">
+        <f xml:space="preserve"> F27 - ABS(C27)</f>
+        <v>-0.30000000000000071</v>
+      </c>
+      <c r="M27">
+        <f xml:space="preserve"> G27 - ABS(D27)</f>
+        <v>0.39999999999999858</v>
+      </c>
+    </row>
+    <row r="28" spans="3:14">
+      <c r="C28" s="1">
+        <v>-35.6</v>
+      </c>
+      <c r="D28" s="1">
+        <v>-47.6</v>
+      </c>
+      <c r="F28">
+        <v>35.5</v>
+      </c>
+      <c r="G28">
+        <v>48</v>
+      </c>
+      <c r="L28">
+        <f xml:space="preserve"> F28 - ABS(C28)</f>
+        <v>-0.10000000000000142</v>
+      </c>
+      <c r="M28">
+        <f t="shared" ref="M28:M33" si="9" xml:space="preserve"> G28 - ABS(D28)</f>
+        <v>0.39999999999999858</v>
+      </c>
+      <c r="N28">
+        <f t="shared" ref="N28:N33" si="10">H28 - ABS(E28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="3:14">
+      <c r="C29" s="1">
+        <v>-41.2</v>
+      </c>
+      <c r="D29" s="1">
+        <v>-47.8</v>
+      </c>
+      <c r="F29">
+        <v>41.25</v>
+      </c>
+      <c r="G29">
+        <v>48</v>
+      </c>
+      <c r="L29">
+        <f xml:space="preserve"> F29 - ABS(C29)</f>
+        <v>4.9999999999997158E-2</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="9"/>
+        <v>0.20000000000000284</v>
+      </c>
+    </row>
+    <row r="30" spans="3:14">
+      <c r="C30" s="1">
+        <v>-41.8</v>
+      </c>
+      <c r="D30" s="1">
+        <v>-37.6</v>
+      </c>
+      <c r="F30">
+        <v>41.25</v>
+      </c>
+      <c r="G30">
+        <v>38</v>
+      </c>
+      <c r="L30">
+        <f xml:space="preserve"> F30 - ABS(C30)</f>
+        <v>-0.54999999999999716</v>
+      </c>
+      <c r="M30">
+        <f xml:space="preserve"> G30 - ABS(D30)</f>
+        <v>0.39999999999999858</v>
+      </c>
+    </row>
+    <row r="31" spans="3:14">
+      <c r="C31" s="1">
+        <v>-35.799999999999997</v>
+      </c>
+      <c r="D31" s="1">
+        <v>-37.6</v>
+      </c>
+      <c r="F31">
+        <v>35.5</v>
+      </c>
+      <c r="G31">
+        <v>38</v>
+      </c>
+      <c r="L31">
+        <f xml:space="preserve"> F31 - ABS(C31)</f>
+        <v>-0.29999999999999716</v>
+      </c>
+      <c r="M31">
+        <f xml:space="preserve"> G31 - ABS(D31)</f>
+        <v>0.39999999999999858</v>
+      </c>
+      <c r="N31">
+        <f t="shared" ref="N31:N33" si="11">H31 - ABS(E31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="3:14">
+      <c r="C32" s="4">
+        <v>-29.1</v>
+      </c>
+      <c r="D32" s="4">
+        <v>-37.6</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <f xml:space="preserve"> F32 - ABS(C32)</f>
+        <v>-29.1</v>
+      </c>
+      <c r="M32">
+        <f xml:space="preserve"> G32 - ABS(D32)</f>
+        <v>-37.6</v>
+      </c>
+    </row>
+    <row r="33" spans="12:14">
+      <c r="L33">
+        <f t="shared" ref="L33" si="12">F33 - ABS( C33)</f>
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <f t="shared" ref="M33" si="13">G33 - ABS(D33)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="12:14">
+      <c r="M39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="12:14">
+      <c r="L41">
+        <f>AVERAGE(L2:L10, L11:L15)</f>
+        <v>-0.31153846153846187</v>
+      </c>
+      <c r="M41">
+        <f>AVERAGE(M2:M10)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="N41">
+        <f>AVERAGE(N2, N4:N8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="12:14">
+      <c r="L43" t="s">
+        <v>64</v>
+      </c>
+      <c r="M43" t="s">
+        <v>62</v>
+      </c>
+      <c r="N43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="12:14">
+      <c r="L44">
+        <f>L2 - $L$41</f>
+        <v>-0.3384615384615367</v>
+      </c>
+      <c r="M44">
+        <f>M2 - $M$41</f>
+        <v>6.6666666666665264E-2</v>
+      </c>
+      <c r="N44">
+        <f>N2 - $N$41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="12:14">
+      <c r="L45">
+        <f>L3 - $L$41</f>
+        <v>0.31153846153846187</v>
+      </c>
+      <c r="M45">
+        <f>M3 - $M$41</f>
+        <v>0.26666666666666811</v>
+      </c>
+      <c r="N45">
+        <f>N3 - $N$41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="12:14">
+      <c r="L46">
+        <f>L4 - $L$41</f>
+        <v>-8.8461538461536704E-2</v>
+      </c>
+      <c r="M46">
+        <f>M4 - $M$41</f>
+        <v>0.26666666666666811</v>
+      </c>
+      <c r="N46">
+        <f>N4 - $N$41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="12:14">
+      <c r="L47">
+        <f>L5 - $L$41</f>
+        <v>-0.28846153846153955</v>
+      </c>
+      <c r="M47">
+        <f>M5 - $M$41</f>
+        <v>6.6666666666665264E-2</v>
+      </c>
+      <c r="N47">
+        <f>N5 - $N$41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="12:14">
+      <c r="L48">
+        <f>L6 - $L$41</f>
+        <v>0.11153846153845903</v>
+      </c>
+      <c r="M48">
+        <f>M6 - $M$41</f>
+        <v>-3.3333333333336157E-2</v>
+      </c>
+      <c r="N48">
+        <f>N6 - $N$41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="12:14">
+      <c r="L49">
+        <f>L7 - $L$41</f>
+        <v>6.1538461538461875E-2</v>
+      </c>
+      <c r="M49">
+        <f>M7 - $M$41</f>
+        <v>-0.13333333333333047</v>
+      </c>
+      <c r="N49">
+        <f>N7 - $N$41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="12:14">
+      <c r="L50">
+        <f>L8 - $L$41</f>
+        <v>0.31153846153846187</v>
+      </c>
+      <c r="M50">
+        <f>M8 - $M$41</f>
+        <v>-3.3333333333336157E-2</v>
+      </c>
+      <c r="N50">
+        <f>N8 - $N$41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="12:14">
+      <c r="L51">
+        <f>L9 - $L$41</f>
+        <v>0.4115384615384633</v>
+      </c>
+      <c r="M51">
+        <f>M9 - $M$41</f>
+        <v>-0.23333333333333189</v>
+      </c>
+    </row>
+    <row r="52" spans="12:14">
+      <c r="L52">
+        <f>L10 - $L$41</f>
+        <v>0.46153846153846045</v>
+      </c>
+      <c r="M52">
+        <f>M10 - $M$41</f>
+        <v>-0.23333333333333189</v>
+      </c>
+    </row>
+    <row r="54" spans="12:14">
+      <c r="L54">
+        <f>L11 - $L$41</f>
+        <v>0.31153846153846187</v>
+      </c>
+      <c r="M54">
+        <f>M11 - $M$41</f>
+        <v>6.6666666666665264E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="12:14">
+      <c r="L55">
+        <f>L12 - $L$41</f>
+        <v>-0.48846153846153884</v>
+      </c>
+      <c r="M55">
+        <f>M12 - $M$41</f>
+        <v>0.36666666666666953</v>
+      </c>
+    </row>
+    <row r="56" spans="12:14">
+      <c r="L56">
+        <f>L13 - $L$41</f>
+        <v>-0.48846153846153884</v>
+      </c>
+      <c r="M56">
+        <f>M13 - $M$41</f>
+        <v>0.26666666666666811</v>
+      </c>
+    </row>
+    <row r="57" spans="12:14">
+      <c r="L57">
+        <f>L14 - $L$41</f>
+        <v>-0.28846153846153955</v>
+      </c>
+      <c r="M57">
+        <f>M14 - $M$41</f>
+        <v>0.56666666666666532</v>
+      </c>
+    </row>
+    <row r="58" spans="12:14">
+      <c r="L58">
+        <f>L15 - $L$41</f>
+        <v>0.31153846153846187</v>
+      </c>
+      <c r="M58">
+        <f>M15 - $M$41</f>
+        <v>-0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="59" spans="12:14">
+      <c r="L59">
+        <f>L17 - $L$41</f>
+        <v>0.31153846153846187</v>
+      </c>
+      <c r="M59">
+        <f>M17 - $M$41</f>
+        <v>-0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="60" spans="12:14">
+      <c r="L60">
+        <f>L18 - $L$41</f>
+        <v>0.31153846153846187</v>
+      </c>
+      <c r="M60">
+        <f>M18 - $M$41</f>
+        <v>-0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="63" spans="12:14">
+      <c r="L63" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="12:13">
+      <c r="L65" t="s">
+        <v>67</v>
+      </c>
+      <c r="M65" s="3">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="66" spans="12:13">
+      <c r="L66" t="s">
+        <v>68</v>
+      </c>
+      <c r="M66" s="3">
+        <v>2.58</v>
+      </c>
+    </row>
+    <row r="68" spans="12:13">
+      <c r="L68" t="s">
+        <v>69</v>
+      </c>
+      <c r="M68">
+        <f>M65+M41</f>
+        <v>0.80333333333333323</v>
+      </c>
+    </row>
+    <row r="69" spans="12:13">
+      <c r="L69" t="s">
+        <v>70</v>
+      </c>
+      <c r="M69">
+        <f>M66+M41</f>
+        <v>2.9133333333333336</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AAEF31-204C-EF4F-9548-47B3CC48B309}">
+  <dimension ref="A1:M23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="1">
+        <v>-28.4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-56.7</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2">
+        <v>28.5</v>
+      </c>
+      <c r="F2">
+        <v>57</v>
+      </c>
+      <c r="K2">
+        <f xml:space="preserve"> E2 - ABS(B2)</f>
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="L2">
+        <f xml:space="preserve"> F2 - ABS(C2)</f>
+        <v>0.29999999999999716</v>
+      </c>
+      <c r="M2">
+        <f xml:space="preserve"> G2 - ABS(D2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-35.4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-56.9</v>
+      </c>
+      <c r="E3">
+        <v>35.5</v>
+      </c>
+      <c r="F3">
+        <v>57</v>
+      </c>
+      <c r="K3">
+        <f xml:space="preserve"> E3 - ABS(B3)</f>
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="L3">
+        <f xml:space="preserve"> F3 - ABS(C3)</f>
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="M3">
+        <f xml:space="preserve"> G3 - ABS(D3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="1">
+        <v>-41.1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-56.9</v>
+      </c>
+      <c r="E4">
+        <v>41.25</v>
+      </c>
+      <c r="F4">
+        <v>57</v>
+      </c>
+      <c r="K4">
+        <f xml:space="preserve"> E4 - ABS(B4)</f>
+        <v>0.14999999999999858</v>
+      </c>
+      <c r="L4">
+        <f xml:space="preserve"> F4 - ABS(C4)</f>
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="M4">
+        <f xml:space="preserve"> G4 - ABS(D4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="1">
+        <v>-28.9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-47.5</v>
+      </c>
+      <c r="E5">
+        <v>28.5</v>
+      </c>
+      <c r="F5">
+        <v>48</v>
+      </c>
+      <c r="K5">
+        <f xml:space="preserve"> E5 - ABS(B5)</f>
+        <v>-0.39999999999999858</v>
+      </c>
+      <c r="L5">
+        <f xml:space="preserve"> F5 - ABS(C5)</f>
+        <v>0.5</v>
+      </c>
+      <c r="M5">
+        <f xml:space="preserve"> G5 - ABS(D5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-35.700000000000003</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-47.7</v>
+      </c>
+      <c r="E6">
+        <v>35.5</v>
+      </c>
+      <c r="F6">
+        <v>48</v>
+      </c>
+      <c r="K6">
+        <f xml:space="preserve"> E6 - ABS(B6)</f>
+        <v>-0.20000000000000284</v>
+      </c>
+      <c r="L6">
+        <f xml:space="preserve"> F6 - ABS(C6)</f>
+        <v>0.29999999999999716</v>
+      </c>
+      <c r="M6">
+        <f xml:space="preserve"> G6 - ABS(D6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="1">
+        <v>-41.3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-47.7</v>
+      </c>
+      <c r="E7">
+        <v>41.25</v>
+      </c>
+      <c r="F7">
+        <v>48</v>
+      </c>
+      <c r="K7">
+        <f xml:space="preserve"> E7 - ABS(B7)</f>
+        <v>-4.9999999999997158E-2</v>
+      </c>
+      <c r="L7">
+        <f xml:space="preserve"> F7 - ABS(C7)</f>
+        <v>0.29999999999999716</v>
+      </c>
+      <c r="M7">
+        <f xml:space="preserve"> G7 - ABS(D7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="1">
+        <v>-29.1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>-37.4</v>
+      </c>
+      <c r="E8">
+        <v>28.5</v>
+      </c>
+      <c r="F8">
+        <v>38</v>
+      </c>
+      <c r="K8">
+        <f xml:space="preserve"> E8 - ABS(B8)</f>
+        <v>-0.60000000000000142</v>
+      </c>
+      <c r="L8">
+        <f xml:space="preserve"> F8 - ABS(C8)</f>
+        <v>0.60000000000000142</v>
+      </c>
+      <c r="M8">
+        <f xml:space="preserve"> G8 - ABS(D8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="1">
+        <v>-35.6</v>
+      </c>
+      <c r="C9" s="1">
+        <v>-37.6</v>
+      </c>
+      <c r="E9">
+        <v>35.5</v>
+      </c>
+      <c r="F9">
+        <v>38</v>
+      </c>
+      <c r="K9">
+        <f xml:space="preserve"> E9 - ABS(B9)</f>
+        <v>-0.10000000000000142</v>
+      </c>
+      <c r="L9">
+        <f xml:space="preserve"> F9 - ABS(C9)</f>
+        <v>0.39999999999999858</v>
+      </c>
+      <c r="M9">
+        <f xml:space="preserve"> G9 - ABS(D9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="1">
+        <v>-41.3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-37.6</v>
+      </c>
+      <c r="E10">
+        <v>41.25</v>
+      </c>
+      <c r="F10">
+        <v>38</v>
+      </c>
+      <c r="K10">
+        <f xml:space="preserve"> E10 - ABS(B10)</f>
+        <v>-4.9999999999997158E-2</v>
+      </c>
+      <c r="L10">
+        <f xml:space="preserve"> F10 - ABS(C10)</f>
+        <v>0.39999999999999858</v>
+      </c>
+      <c r="M10">
+        <f xml:space="preserve"> G10 - ABS(D10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="1">
+        <v>-29.3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-27.2</v>
+      </c>
+      <c r="E12">
+        <v>28.5</v>
+      </c>
+      <c r="F12">
+        <v>28</v>
+      </c>
+      <c r="K12">
+        <f t="shared" ref="K11:K12" si="0" xml:space="preserve"> E12 - ABS(B12)</f>
+        <v>-0.80000000000000071</v>
+      </c>
+      <c r="L12">
+        <f t="shared" ref="L11:L12" si="1" xml:space="preserve"> F12 - ABS(C12)</f>
+        <v>0.80000000000000071</v>
+      </c>
+      <c r="M12">
+        <f t="shared" ref="M11:M12" si="2" xml:space="preserve"> G12 - ABS(D12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="1">
+        <v>-36.299999999999997</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-27.4</v>
+      </c>
+      <c r="E13">
+        <v>35.5</v>
+      </c>
+      <c r="F13">
+        <v>28</v>
+      </c>
+      <c r="K13">
+        <f t="shared" ref="K13" si="3" xml:space="preserve"> E13 - ABS(B13)</f>
+        <v>-0.79999999999999716</v>
+      </c>
+      <c r="L13">
+        <f t="shared" ref="L13" si="4" xml:space="preserve"> F13 - ABS(C13)</f>
+        <v>0.60000000000000142</v>
+      </c>
+      <c r="M13">
+        <f t="shared" ref="M13" si="5" xml:space="preserve"> G13 - ABS(D13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="1">
+        <v>-41.8</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-27.5</v>
+      </c>
+      <c r="E14">
+        <v>41.25</v>
+      </c>
+      <c r="F14">
+        <v>28</v>
+      </c>
+      <c r="K14">
+        <f t="shared" ref="K14" si="6" xml:space="preserve"> E14 - ABS(B14)</f>
+        <v>-0.54999999999999716</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ref="L14" si="7" xml:space="preserve"> F14 - ABS(C14)</f>
+        <v>0.5</v>
+      </c>
+      <c r="M14">
+        <f t="shared" ref="M14" si="8" xml:space="preserve"> G14 - ABS(D14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="1">
+        <v>-35.200000000000003</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="E16">
+        <v>35.5</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <f t="shared" ref="K15:K17" si="9" xml:space="preserve"> E16 - ABS(B16)</f>
+        <v>0.29999999999999716</v>
+      </c>
+      <c r="L16">
+        <f t="shared" ref="L15:L17" si="10" xml:space="preserve"> F16 - ABS(C16)</f>
+        <v>-1.2</v>
+      </c>
+      <c r="M16">
+        <f t="shared" ref="M15:M16" si="11" xml:space="preserve"> G16 - ABS(D16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="1">
+        <v>-35.799999999999997</v>
+      </c>
+      <c r="C17" s="1">
+        <v>-9.1</v>
+      </c>
+      <c r="E17">
+        <v>35.5</v>
+      </c>
+      <c r="F17">
+        <v>10</v>
+      </c>
+      <c r="K17">
+        <f xml:space="preserve"> E17 - ABS(B17)</f>
+        <v>-0.29999999999999716</v>
+      </c>
+      <c r="L17">
+        <f xml:space="preserve"> F17 - ABS(C17)</f>
+        <v>0.90000000000000036</v>
+      </c>
+      <c r="M17">
+        <f t="shared" ref="M17" si="12" xml:space="preserve"> G17 - ABS(D17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21">
+        <v>18</v>
+      </c>
+      <c r="F21">
+        <v>48</v>
+      </c>
+      <c r="K21">
+        <f t="shared" ref="K18:K23" si="13" xml:space="preserve"> E21 - ABS(B21)</f>
+        <v>18</v>
+      </c>
+      <c r="L21">
+        <f t="shared" ref="L18:L23" si="14" xml:space="preserve"> F21 - ABS(C21)</f>
+        <v>48</v>
+      </c>
+      <c r="M21">
+        <f t="shared" ref="M18:M23" si="15" xml:space="preserve"> G21 - ABS(D21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22">
+        <v>18</v>
+      </c>
+      <c r="F22">
+        <v>38</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="13"/>
+        <v>18</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="14"/>
+        <v>38</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="1">
+        <v>-18.3</v>
+      </c>
+      <c r="C23" s="1">
+        <v>-28.5</v>
+      </c>
+      <c r="E23">
+        <v>18</v>
+      </c>
+      <c r="F23">
+        <v>28</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="13"/>
+        <v>-0.30000000000000071</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="14"/>
+        <v>-0.5</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Some Vision Data showing a fudge factor for the robot _make a clean field_)
</commit_message>
<xml_diff>
--- a/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
+++ b/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/Dropbox/Brain Stormz FTC/2023-24-code/AprilTag Performance Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF8A3E3-BA1E-F44D-A360-315012DE6214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A2110A-2A91-EC4E-B69C-CD10C7600318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="100">
   <si>
     <t>Point</t>
   </si>
@@ -307,6 +308,39 @@
   </si>
   <si>
     <t>(1,0)</t>
+  </si>
+  <si>
+    <t>B(2, 3)</t>
+  </si>
+  <si>
+    <t>B(2, 2)</t>
+  </si>
+  <si>
+    <t>B(2, 1)</t>
+  </si>
+  <si>
+    <t>B(0, 3)</t>
+  </si>
+  <si>
+    <t>Real X (TAG REL)</t>
+  </si>
+  <si>
+    <t>B(1, 3)</t>
+  </si>
+  <si>
+    <t>B(0, 2)</t>
+  </si>
+  <si>
+    <t>B(1, 2)</t>
+  </si>
+  <si>
+    <t>B(0, 1)</t>
+  </si>
+  <si>
+    <t>B(1, 1)</t>
+  </si>
+  <si>
+    <t>Fudge Factor:</t>
   </si>
 </sst>
 </file>
@@ -3272,8 +3306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AAEF31-204C-EF4F-9548-47B3CC48B309}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3715,6 +3749,12 @@
       <c r="A21" t="s">
         <v>88</v>
       </c>
+      <c r="B21" s="1">
+        <v>-17.8</v>
+      </c>
+      <c r="C21" s="1">
+        <v>-48</v>
+      </c>
       <c r="E21">
         <v>18</v>
       </c>
@@ -3723,11 +3763,11 @@
       </c>
       <c r="K21">
         <f t="shared" ref="K18:K23" si="13" xml:space="preserve"> E21 - ABS(B21)</f>
-        <v>18</v>
+        <v>0.19999999999999929</v>
       </c>
       <c r="L21">
         <f t="shared" ref="L18:L23" si="14" xml:space="preserve"> F21 - ABS(C21)</f>
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="M21">
         <f t="shared" ref="M18:M23" si="15" xml:space="preserve"> G21 - ABS(D21)</f>
@@ -3738,6 +3778,12 @@
       <c r="A22" t="s">
         <v>87</v>
       </c>
+      <c r="B22" s="1">
+        <v>-18.100000000000001</v>
+      </c>
+      <c r="C22" s="1">
+        <v>-37.700000000000003</v>
+      </c>
       <c r="E22">
         <v>18</v>
       </c>
@@ -3746,11 +3792,11 @@
       </c>
       <c r="K22">
         <f t="shared" si="13"/>
-        <v>18</v>
+        <v>-0.10000000000000142</v>
       </c>
       <c r="L22">
         <f t="shared" si="14"/>
-        <v>38</v>
+        <v>0.29999999999999716</v>
       </c>
       <c r="M22">
         <f t="shared" si="15"/>
@@ -3784,6 +3830,411 @@
       <c r="M23">
         <f t="shared" si="15"/>
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C249CE-14E9-E34F-BB7C-65B8ECA9DC1D}">
+  <dimension ref="A1:M32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="1">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-38.6</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2">
+        <v>28</v>
+      </c>
+      <c r="F2">
+        <v>39</v>
+      </c>
+      <c r="K2">
+        <f xml:space="preserve"> E2 - ABS(B2)</f>
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <f xml:space="preserve"> F2 - ABS(C2)</f>
+        <v>0.39999999999999858</v>
+      </c>
+      <c r="M2">
+        <f xml:space="preserve"> G2 - ABS(D2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="1">
+        <v>34.6</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-38.5</v>
+      </c>
+      <c r="E3">
+        <v>35.5</v>
+      </c>
+      <c r="F3">
+        <v>39</v>
+      </c>
+      <c r="K3">
+        <f xml:space="preserve"> E3 - ABS(B3)</f>
+        <v>0.89999999999999858</v>
+      </c>
+      <c r="L3">
+        <f xml:space="preserve"> F3 - ABS(C3)</f>
+        <v>0.5</v>
+      </c>
+      <c r="M3">
+        <f xml:space="preserve"> G3 - ABS(D3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="1">
+        <v>41.7</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-37.799999999999997</v>
+      </c>
+      <c r="E4">
+        <v>43</v>
+      </c>
+      <c r="F4">
+        <v>38.5</v>
+      </c>
+      <c r="K4">
+        <f xml:space="preserve"> E4 - ABS(B4)</f>
+        <v>1.2999999999999972</v>
+      </c>
+      <c r="L4">
+        <f xml:space="preserve"> F4 - ABS(C4)</f>
+        <v>0.70000000000000284</v>
+      </c>
+      <c r="M4">
+        <f xml:space="preserve"> G4 - ABS(D4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ref="K5:K8" si="0" xml:space="preserve"> E7 - ABS(B7)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="L7">
+        <f t="shared" ref="L5:L8" si="1" xml:space="preserve"> F7 - ABS(C7)</f>
+        <v>-0.69999999999999929</v>
+      </c>
+      <c r="M7">
+        <f t="shared" ref="M5:M8" si="2" xml:space="preserve"> G7 - ABS(D7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>14.8</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>14</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>-0.1</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>-0.80000000000000071</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>24.9</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>24</v>
+      </c>
+      <c r="K9">
+        <f t="shared" ref="K9" si="3" xml:space="preserve"> E9 - ABS(B9)</f>
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <f t="shared" ref="L9" si="4" xml:space="preserve"> F9 - ABS(C9)</f>
+        <v>-0.89999999999999858</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ref="M9" si="5" xml:space="preserve"> G9 - ABS(D9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>8.25</v>
+      </c>
+      <c r="K10">
+        <f t="shared" ref="K10:K11" si="6" xml:space="preserve"> E10 - ABS(B10)</f>
+        <v>-0.1</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ref="L10:L11" si="7" xml:space="preserve"> F10 - ABS(C10)</f>
+        <v>-0.55000000000000071</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ref="M10" si="8" xml:space="preserve"> G10 - ABS(D10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="1">
+        <v>-0.3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>14.9</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>14.25</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="6"/>
+        <v>-0.3</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="7"/>
+        <v>-0.65000000000000036</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="1">
+        <v>-0.6</v>
+      </c>
+      <c r="C12" s="1">
+        <v>25</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>24.5</v>
+      </c>
+      <c r="K12">
+        <f t="shared" ref="K12" si="9" xml:space="preserve"> E12 - ABS(B12)</f>
+        <v>-0.6</v>
+      </c>
+      <c r="L12">
+        <f t="shared" ref="L12" si="10" xml:space="preserve"> F12 - ABS(C12)</f>
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>9</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>8</v>
+      </c>
+      <c r="K13">
+        <f t="shared" ref="K13" si="11" xml:space="preserve"> E13 - ABS(B13)</f>
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f t="shared" ref="L13" si="12" xml:space="preserve"> F13 - ABS(C13)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>15</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="L16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="12:13">
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <f>AVERAGE(L2:L4, L7:L13)</f>
+        <v>-0.34999999999999981</v>
+      </c>
+    </row>
+    <row r="22" spans="12:13">
+      <c r="L22">
+        <f>L2-$M$20</f>
+        <v>0.74999999999999845</v>
+      </c>
+    </row>
+    <row r="23" spans="12:13">
+      <c r="L23">
+        <f t="shared" ref="L23:L32" si="13">L3-$M$20</f>
+        <v>0.84999999999999987</v>
+      </c>
+    </row>
+    <row r="24" spans="12:13">
+      <c r="L24">
+        <f>L4-$M$20</f>
+        <v>1.0500000000000027</v>
+      </c>
+    </row>
+    <row r="27" spans="12:13">
+      <c r="L27">
+        <f>L7-$M$20</f>
+        <v>-0.34999999999999948</v>
+      </c>
+    </row>
+    <row r="28" spans="12:13">
+      <c r="L28">
+        <f t="shared" si="13"/>
+        <v>-0.4500000000000009</v>
+      </c>
+    </row>
+    <row r="29" spans="12:13">
+      <c r="L29">
+        <f t="shared" si="13"/>
+        <v>-0.54999999999999871</v>
+      </c>
+    </row>
+    <row r="30" spans="12:13">
+      <c r="L30">
+        <f t="shared" si="13"/>
+        <v>-0.2000000000000009</v>
+      </c>
+    </row>
+    <row r="31" spans="12:13">
+      <c r="L31">
+        <f t="shared" si="13"/>
+        <v>-0.30000000000000054</v>
+      </c>
+    </row>
+    <row r="32" spans="12:13">
+      <c r="L32">
+        <f t="shared" si="13"/>
+        <v>-0.15000000000000019</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds Second Set of Error Factors And Cutoff for One Inch Accuracy into Apriltag
</commit_message>
<xml_diff>
--- a/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
+++ b/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/Dropbox/Brain Stormz FTC/2023-24-code/AprilTag Performance Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A2110A-2A91-EC4E-B69C-CD10C7600318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EFADD4-A4E3-0249-9F25-B2ACE35EBC5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="6" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="107">
   <si>
     <t>Point</t>
   </si>
@@ -341,13 +342,34 @@
   </si>
   <si>
     <t>Fudge Factor:</t>
+  </si>
+  <si>
+    <t>A(0, 2)</t>
+  </si>
+  <si>
+    <t>B(0,2)</t>
+  </si>
+  <si>
+    <t>B(0,3)</t>
+  </si>
+  <si>
+    <t>B(0,1)</t>
+  </si>
+  <si>
+    <t>AVG Y ERR</t>
+  </si>
+  <si>
+    <t>AVG X ERR -&gt;</t>
+  </si>
+  <si>
+    <t>ADJUSTED Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -374,6 +396,12 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF7A7E85"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -395,13 +423,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2096,7 +2128,7 @@
     </row>
     <row r="24" spans="12:14">
       <c r="L24">
-        <f>L2 - $L$21</f>
+        <f t="shared" ref="L24:L32" si="6">L2 - $L$21</f>
         <v>-0.33392857142856969</v>
       </c>
       <c r="M24">
@@ -2110,105 +2142,105 @@
     </row>
     <row r="25" spans="12:14">
       <c r="L25">
-        <f>L3 - $L$21</f>
+        <f t="shared" si="6"/>
         <v>0.31607142857142889</v>
       </c>
       <c r="M25">
-        <f t="shared" ref="M25:M40" si="6">M3 - $M$21</f>
+        <f t="shared" ref="M25:M40" si="7">M3 - $M$21</f>
         <v>0.26666666666666811</v>
       </c>
       <c r="N25">
-        <f t="shared" ref="N25:N30" si="7">N3 - $N$21</f>
+        <f t="shared" ref="N25:N30" si="8">N3 - $N$21</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="12:14">
       <c r="L26">
-        <f>L4 - $L$21</f>
+        <f t="shared" si="6"/>
         <v>-8.3928571428569687E-2</v>
       </c>
       <c r="M26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.26666666666666811</v>
       </c>
       <c r="N26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="12:14">
       <c r="L27">
-        <f>L5 - $L$21</f>
+        <f t="shared" si="6"/>
         <v>-0.28392857142857253</v>
       </c>
       <c r="M27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.6666666666665264E-2</v>
       </c>
       <c r="N27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="12:14">
       <c r="L28">
-        <f>L6 - $L$21</f>
+        <f t="shared" si="6"/>
         <v>0.11607142857142605</v>
       </c>
       <c r="M28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-3.3333333333336157E-2</v>
       </c>
       <c r="N28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="12:14">
       <c r="L29">
-        <f>L7 - $L$21</f>
+        <f t="shared" si="6"/>
         <v>6.6071428571428892E-2</v>
       </c>
       <c r="M29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.13333333333333047</v>
       </c>
       <c r="N29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="12:14">
       <c r="L30">
-        <f>L8 - $L$21</f>
+        <f t="shared" si="6"/>
         <v>0.31607142857142889</v>
       </c>
       <c r="M30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-3.3333333333336157E-2</v>
       </c>
       <c r="N30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="12:14">
       <c r="L31">
-        <f>L9 - $L$21</f>
+        <f t="shared" si="6"/>
         <v>0.41607142857143031</v>
       </c>
       <c r="M31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.23333333333333189</v>
       </c>
     </row>
     <row r="32" spans="12:14">
       <c r="L32">
-        <f>L10 - $L$21</f>
+        <f t="shared" si="6"/>
         <v>0.46607142857142747</v>
       </c>
       <c r="M32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.23333333333333189</v>
       </c>
     </row>
@@ -2268,7 +2300,7 @@
         <v>0.31607142857142889</v>
       </c>
       <c r="M39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.33333333333333331</v>
       </c>
     </row>
@@ -2278,7 +2310,7 @@
         <v>0.31607142857142889</v>
       </c>
       <c r="M40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.33333333333333331</v>
       </c>
     </row>
@@ -2794,7 +2826,7 @@
         <v>2.7000000000000028</v>
       </c>
       <c r="N22">
-        <f t="shared" ref="N22:N33" si="5">H22 - ABS(E22)</f>
+        <f t="shared" ref="N22" si="5">H22 - ABS(E22)</f>
         <v>0</v>
       </c>
     </row>
@@ -2812,11 +2844,11 @@
         <v>48</v>
       </c>
       <c r="L23">
-        <f xml:space="preserve"> F23 - ABS(C23)</f>
+        <f t="shared" ref="L23:L32" si="6" xml:space="preserve"> F23 - ABS(C23)</f>
         <v>4.9999999999997158E-2</v>
       </c>
       <c r="M23">
-        <f t="shared" ref="M22:M33" si="6" xml:space="preserve"> G23 - ABS(D23)</f>
+        <f t="shared" ref="M23" si="7" xml:space="preserve"> G23 - ABS(D23)</f>
         <v>0.20000000000000284</v>
       </c>
     </row>
@@ -2834,7 +2866,7 @@
         <v>57</v>
       </c>
       <c r="L24">
-        <f xml:space="preserve"> F24 - ABS(C24)</f>
+        <f t="shared" si="6"/>
         <v>0.25</v>
       </c>
       <c r="M24">
@@ -2856,15 +2888,15 @@
         <v>57</v>
       </c>
       <c r="L25">
-        <f xml:space="preserve"> F25 - ABS(C25)</f>
+        <f t="shared" si="6"/>
         <v>0.10000000000000142</v>
       </c>
       <c r="M25">
-        <f t="shared" ref="M25:M33" si="7" xml:space="preserve"> G25 - ABS(D25)</f>
+        <f t="shared" ref="M25:M26" si="8" xml:space="preserve"> G25 - ABS(D25)</f>
         <v>0.10000000000000142</v>
       </c>
       <c r="N25">
-        <f t="shared" ref="N25:N33" si="8">H25 - ABS(E25)</f>
+        <f t="shared" ref="N25" si="9">H25 - ABS(E25)</f>
         <v>0</v>
       </c>
     </row>
@@ -2882,11 +2914,11 @@
         <v>57</v>
       </c>
       <c r="L26">
-        <f xml:space="preserve"> F26 - ABS(C26)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.29999999999999716</v>
       </c>
     </row>
@@ -2904,7 +2936,7 @@
         <v>48</v>
       </c>
       <c r="L27">
-        <f xml:space="preserve"> F27 - ABS(C27)</f>
+        <f t="shared" si="6"/>
         <v>-0.30000000000000071</v>
       </c>
       <c r="M27">
@@ -2926,15 +2958,15 @@
         <v>48</v>
       </c>
       <c r="L28">
-        <f xml:space="preserve"> F28 - ABS(C28)</f>
+        <f t="shared" si="6"/>
         <v>-0.10000000000000142</v>
       </c>
       <c r="M28">
-        <f t="shared" ref="M28:M33" si="9" xml:space="preserve"> G28 - ABS(D28)</f>
+        <f t="shared" ref="M28:M29" si="10" xml:space="preserve"> G28 - ABS(D28)</f>
         <v>0.39999999999999858</v>
       </c>
       <c r="N28">
-        <f t="shared" ref="N28:N33" si="10">H28 - ABS(E28)</f>
+        <f t="shared" ref="N28" si="11">H28 - ABS(E28)</f>
         <v>0</v>
       </c>
     </row>
@@ -2952,11 +2984,11 @@
         <v>48</v>
       </c>
       <c r="L29">
-        <f xml:space="preserve"> F29 - ABS(C29)</f>
+        <f t="shared" si="6"/>
         <v>4.9999999999997158E-2</v>
       </c>
       <c r="M29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.20000000000000284</v>
       </c>
     </row>
@@ -2974,7 +3006,7 @@
         <v>38</v>
       </c>
       <c r="L30">
-        <f xml:space="preserve"> F30 - ABS(C30)</f>
+        <f t="shared" si="6"/>
         <v>-0.54999999999999716</v>
       </c>
       <c r="M30">
@@ -2996,7 +3028,7 @@
         <v>38</v>
       </c>
       <c r="L31">
-        <f xml:space="preserve"> F31 - ABS(C31)</f>
+        <f t="shared" si="6"/>
         <v>-0.29999999999999716</v>
       </c>
       <c r="M31">
@@ -3004,7 +3036,7 @@
         <v>0.39999999999999858</v>
       </c>
       <c r="N31">
-        <f t="shared" ref="N31:N33" si="11">H31 - ABS(E31)</f>
+        <f t="shared" ref="N31" si="12">H31 - ABS(E31)</f>
         <v>0</v>
       </c>
     </row>
@@ -3022,7 +3054,7 @@
         <v>0</v>
       </c>
       <c r="L32">
-        <f xml:space="preserve"> F32 - ABS(C32)</f>
+        <f t="shared" si="6"/>
         <v>-29.1</v>
       </c>
       <c r="M32">
@@ -3032,11 +3064,11 @@
     </row>
     <row r="33" spans="12:14">
       <c r="L33">
-        <f t="shared" ref="L33" si="12">F33 - ABS( C33)</f>
+        <f t="shared" ref="L33" si="13">F33 - ABS( C33)</f>
         <v>0</v>
       </c>
       <c r="M33">
-        <f t="shared" ref="M33" si="13">G33 - ABS(D33)</f>
+        <f t="shared" ref="M33" si="14">G33 - ABS(D33)</f>
         <v>0</v>
       </c>
     </row>
@@ -3072,119 +3104,119 @@
     </row>
     <row r="44" spans="12:14">
       <c r="L44">
-        <f>L2 - $L$41</f>
+        <f t="shared" ref="L44:L52" si="15">L2 - $L$41</f>
         <v>-0.3384615384615367</v>
       </c>
       <c r="M44">
-        <f>M2 - $M$41</f>
+        <f t="shared" ref="M44:M52" si="16">M2 - $M$41</f>
         <v>6.6666666666665264E-2</v>
       </c>
       <c r="N44">
-        <f>N2 - $N$41</f>
+        <f t="shared" ref="N44:N50" si="17">N2 - $N$41</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="12:14">
       <c r="L45">
-        <f>L3 - $L$41</f>
+        <f t="shared" si="15"/>
         <v>0.31153846153846187</v>
       </c>
       <c r="M45">
-        <f>M3 - $M$41</f>
+        <f t="shared" si="16"/>
         <v>0.26666666666666811</v>
       </c>
       <c r="N45">
-        <f>N3 - $N$41</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="12:14">
       <c r="L46">
-        <f>L4 - $L$41</f>
+        <f t="shared" si="15"/>
         <v>-8.8461538461536704E-2</v>
       </c>
       <c r="M46">
-        <f>M4 - $M$41</f>
+        <f t="shared" si="16"/>
         <v>0.26666666666666811</v>
       </c>
       <c r="N46">
-        <f>N4 - $N$41</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="12:14">
       <c r="L47">
-        <f>L5 - $L$41</f>
+        <f t="shared" si="15"/>
         <v>-0.28846153846153955</v>
       </c>
       <c r="M47">
-        <f>M5 - $M$41</f>
+        <f t="shared" si="16"/>
         <v>6.6666666666665264E-2</v>
       </c>
       <c r="N47">
-        <f>N5 - $N$41</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="12:14">
       <c r="L48">
-        <f>L6 - $L$41</f>
+        <f t="shared" si="15"/>
         <v>0.11153846153845903</v>
       </c>
       <c r="M48">
-        <f>M6 - $M$41</f>
+        <f t="shared" si="16"/>
         <v>-3.3333333333336157E-2</v>
       </c>
       <c r="N48">
-        <f>N6 - $N$41</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="12:14">
       <c r="L49">
-        <f>L7 - $L$41</f>
+        <f t="shared" si="15"/>
         <v>6.1538461538461875E-2</v>
       </c>
       <c r="M49">
-        <f>M7 - $M$41</f>
+        <f t="shared" si="16"/>
         <v>-0.13333333333333047</v>
       </c>
       <c r="N49">
-        <f>N7 - $N$41</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="12:14">
       <c r="L50">
-        <f>L8 - $L$41</f>
+        <f t="shared" si="15"/>
         <v>0.31153846153846187</v>
       </c>
       <c r="M50">
-        <f>M8 - $M$41</f>
+        <f t="shared" si="16"/>
         <v>-3.3333333333336157E-2</v>
       </c>
       <c r="N50">
-        <f>N8 - $N$41</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="12:14">
       <c r="L51">
-        <f>L9 - $L$41</f>
+        <f t="shared" si="15"/>
         <v>0.4115384615384633</v>
       </c>
       <c r="M51">
-        <f>M9 - $M$41</f>
+        <f t="shared" si="16"/>
         <v>-0.23333333333333189</v>
       </c>
     </row>
     <row r="52" spans="12:14">
       <c r="L52">
-        <f>L10 - $L$41</f>
+        <f t="shared" si="15"/>
         <v>0.46153846153846045</v>
       </c>
       <c r="M52">
-        <f>M10 - $M$41</f>
+        <f t="shared" si="16"/>
         <v>-0.23333333333333189</v>
       </c>
     </row>
@@ -3356,15 +3388,15 @@
         <v>57</v>
       </c>
       <c r="K2">
-        <f xml:space="preserve"> E2 - ABS(B2)</f>
+        <f t="shared" ref="K2:K10" si="0" xml:space="preserve"> E2 - ABS(B2)</f>
         <v>0.10000000000000142</v>
       </c>
       <c r="L2">
-        <f xml:space="preserve"> F2 - ABS(C2)</f>
+        <f t="shared" ref="L2:L10" si="1" xml:space="preserve"> F2 - ABS(C2)</f>
         <v>0.29999999999999716</v>
       </c>
       <c r="M2">
-        <f xml:space="preserve"> G2 - ABS(D2)</f>
+        <f t="shared" ref="M2:M10" si="2" xml:space="preserve"> G2 - ABS(D2)</f>
         <v>0</v>
       </c>
     </row>
@@ -3385,15 +3417,15 @@
         <v>57</v>
       </c>
       <c r="K3">
-        <f xml:space="preserve"> E3 - ABS(B3)</f>
+        <f t="shared" si="0"/>
         <v>0.10000000000000142</v>
       </c>
       <c r="L3">
-        <f xml:space="preserve"> F3 - ABS(C3)</f>
+        <f t="shared" si="1"/>
         <v>0.10000000000000142</v>
       </c>
       <c r="M3">
-        <f xml:space="preserve"> G3 - ABS(D3)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3414,15 +3446,15 @@
         <v>57</v>
       </c>
       <c r="K4">
-        <f xml:space="preserve"> E4 - ABS(B4)</f>
+        <f t="shared" si="0"/>
         <v>0.14999999999999858</v>
       </c>
       <c r="L4">
-        <f xml:space="preserve"> F4 - ABS(C4)</f>
+        <f t="shared" si="1"/>
         <v>0.10000000000000142</v>
       </c>
       <c r="M4">
-        <f xml:space="preserve"> G4 - ABS(D4)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3443,15 +3475,15 @@
         <v>48</v>
       </c>
       <c r="K5">
-        <f xml:space="preserve"> E5 - ABS(B5)</f>
+        <f t="shared" si="0"/>
         <v>-0.39999999999999858</v>
       </c>
       <c r="L5">
-        <f xml:space="preserve"> F5 - ABS(C5)</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="M5">
-        <f xml:space="preserve"> G5 - ABS(D5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3472,15 +3504,15 @@
         <v>48</v>
       </c>
       <c r="K6">
-        <f xml:space="preserve"> E6 - ABS(B6)</f>
+        <f t="shared" si="0"/>
         <v>-0.20000000000000284</v>
       </c>
       <c r="L6">
-        <f xml:space="preserve"> F6 - ABS(C6)</f>
+        <f t="shared" si="1"/>
         <v>0.29999999999999716</v>
       </c>
       <c r="M6">
-        <f xml:space="preserve"> G6 - ABS(D6)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3501,15 +3533,15 @@
         <v>48</v>
       </c>
       <c r="K7">
-        <f xml:space="preserve"> E7 - ABS(B7)</f>
+        <f t="shared" si="0"/>
         <v>-4.9999999999997158E-2</v>
       </c>
       <c r="L7">
-        <f xml:space="preserve"> F7 - ABS(C7)</f>
+        <f t="shared" si="1"/>
         <v>0.29999999999999716</v>
       </c>
       <c r="M7">
-        <f xml:space="preserve"> G7 - ABS(D7)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3530,15 +3562,15 @@
         <v>38</v>
       </c>
       <c r="K8">
-        <f xml:space="preserve"> E8 - ABS(B8)</f>
+        <f t="shared" si="0"/>
         <v>-0.60000000000000142</v>
       </c>
       <c r="L8">
-        <f xml:space="preserve"> F8 - ABS(C8)</f>
+        <f t="shared" si="1"/>
         <v>0.60000000000000142</v>
       </c>
       <c r="M8">
-        <f xml:space="preserve"> G8 - ABS(D8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3559,15 +3591,15 @@
         <v>38</v>
       </c>
       <c r="K9">
-        <f xml:space="preserve"> E9 - ABS(B9)</f>
+        <f t="shared" si="0"/>
         <v>-0.10000000000000142</v>
       </c>
       <c r="L9">
-        <f xml:space="preserve"> F9 - ABS(C9)</f>
+        <f t="shared" si="1"/>
         <v>0.39999999999999858</v>
       </c>
       <c r="M9">
-        <f xml:space="preserve"> G9 - ABS(D9)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3588,15 +3620,15 @@
         <v>38</v>
       </c>
       <c r="K10">
-        <f xml:space="preserve"> E10 - ABS(B10)</f>
+        <f t="shared" si="0"/>
         <v>-4.9999999999997158E-2</v>
       </c>
       <c r="L10">
-        <f xml:space="preserve"> F10 - ABS(C10)</f>
+        <f t="shared" si="1"/>
         <v>0.39999999999999858</v>
       </c>
       <c r="M10">
-        <f xml:space="preserve"> G10 - ABS(D10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3617,15 +3649,15 @@
         <v>28</v>
       </c>
       <c r="K12">
-        <f t="shared" ref="K11:K12" si="0" xml:space="preserve"> E12 - ABS(B12)</f>
+        <f t="shared" ref="K12" si="3" xml:space="preserve"> E12 - ABS(B12)</f>
         <v>-0.80000000000000071</v>
       </c>
       <c r="L12">
-        <f t="shared" ref="L11:L12" si="1" xml:space="preserve"> F12 - ABS(C12)</f>
+        <f t="shared" ref="L12" si="4" xml:space="preserve"> F12 - ABS(C12)</f>
         <v>0.80000000000000071</v>
       </c>
       <c r="M12">
-        <f t="shared" ref="M11:M12" si="2" xml:space="preserve"> G12 - ABS(D12)</f>
+        <f t="shared" ref="M12" si="5" xml:space="preserve"> G12 - ABS(D12)</f>
         <v>0</v>
       </c>
     </row>
@@ -3646,15 +3678,15 @@
         <v>28</v>
       </c>
       <c r="K13">
-        <f t="shared" ref="K13" si="3" xml:space="preserve"> E13 - ABS(B13)</f>
+        <f t="shared" ref="K13" si="6" xml:space="preserve"> E13 - ABS(B13)</f>
         <v>-0.79999999999999716</v>
       </c>
       <c r="L13">
-        <f t="shared" ref="L13" si="4" xml:space="preserve"> F13 - ABS(C13)</f>
+        <f t="shared" ref="L13" si="7" xml:space="preserve"> F13 - ABS(C13)</f>
         <v>0.60000000000000142</v>
       </c>
       <c r="M13">
-        <f t="shared" ref="M13" si="5" xml:space="preserve"> G13 - ABS(D13)</f>
+        <f t="shared" ref="M13" si="8" xml:space="preserve"> G13 - ABS(D13)</f>
         <v>0</v>
       </c>
     </row>
@@ -3675,15 +3707,15 @@
         <v>28</v>
       </c>
       <c r="K14">
-        <f t="shared" ref="K14" si="6" xml:space="preserve"> E14 - ABS(B14)</f>
+        <f t="shared" ref="K14" si="9" xml:space="preserve"> E14 - ABS(B14)</f>
         <v>-0.54999999999999716</v>
       </c>
       <c r="L14">
-        <f t="shared" ref="L14" si="7" xml:space="preserve"> F14 - ABS(C14)</f>
+        <f t="shared" ref="L14" si="10" xml:space="preserve"> F14 - ABS(C14)</f>
         <v>0.5</v>
       </c>
       <c r="M14">
-        <f t="shared" ref="M14" si="8" xml:space="preserve"> G14 - ABS(D14)</f>
+        <f t="shared" ref="M14" si="11" xml:space="preserve"> G14 - ABS(D14)</f>
         <v>0</v>
       </c>
     </row>
@@ -3704,15 +3736,15 @@
         <v>0</v>
       </c>
       <c r="K16">
-        <f t="shared" ref="K15:K17" si="9" xml:space="preserve"> E16 - ABS(B16)</f>
+        <f t="shared" ref="K16" si="12" xml:space="preserve"> E16 - ABS(B16)</f>
         <v>0.29999999999999716</v>
       </c>
       <c r="L16">
-        <f t="shared" ref="L15:L17" si="10" xml:space="preserve"> F16 - ABS(C16)</f>
+        <f t="shared" ref="L16" si="13" xml:space="preserve"> F16 - ABS(C16)</f>
         <v>-1.2</v>
       </c>
       <c r="M16">
-        <f t="shared" ref="M15:M16" si="11" xml:space="preserve"> G16 - ABS(D16)</f>
+        <f t="shared" ref="M16" si="14" xml:space="preserve"> G16 - ABS(D16)</f>
         <v>0</v>
       </c>
     </row>
@@ -3741,7 +3773,7 @@
         <v>0.90000000000000036</v>
       </c>
       <c r="M17">
-        <f t="shared" ref="M17" si="12" xml:space="preserve"> G17 - ABS(D17)</f>
+        <f t="shared" ref="M17" si="15" xml:space="preserve"> G17 - ABS(D17)</f>
         <v>0</v>
       </c>
     </row>
@@ -3762,15 +3794,15 @@
         <v>48</v>
       </c>
       <c r="K21">
-        <f t="shared" ref="K18:K23" si="13" xml:space="preserve"> E21 - ABS(B21)</f>
+        <f t="shared" ref="K21:K23" si="16" xml:space="preserve"> E21 - ABS(B21)</f>
         <v>0.19999999999999929</v>
       </c>
       <c r="L21">
-        <f t="shared" ref="L18:L23" si="14" xml:space="preserve"> F21 - ABS(C21)</f>
+        <f t="shared" ref="L21:L23" si="17" xml:space="preserve"> F21 - ABS(C21)</f>
         <v>0</v>
       </c>
       <c r="M21">
-        <f t="shared" ref="M18:M23" si="15" xml:space="preserve"> G21 - ABS(D21)</f>
+        <f t="shared" ref="M21:M23" si="18" xml:space="preserve"> G21 - ABS(D21)</f>
         <v>0</v>
       </c>
     </row>
@@ -3791,15 +3823,15 @@
         <v>38</v>
       </c>
       <c r="K22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>-0.10000000000000142</v>
       </c>
       <c r="L22">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.29999999999999716</v>
       </c>
       <c r="M22">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -3820,15 +3852,15 @@
         <v>28</v>
       </c>
       <c r="K23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>-0.30000000000000071</v>
       </c>
       <c r="L23">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>-0.5</v>
       </c>
       <c r="M23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -3841,8 +3873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C249CE-14E9-E34F-BB7C-65B8ECA9DC1D}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3891,15 +3923,15 @@
         <v>39</v>
       </c>
       <c r="K2">
-        <f xml:space="preserve"> E2 - ABS(B2)</f>
+        <f t="shared" ref="K2:M4" si="0" xml:space="preserve"> E2 - ABS(B2)</f>
         <v>1</v>
       </c>
       <c r="L2">
-        <f xml:space="preserve"> F2 - ABS(C2)</f>
+        <f t="shared" si="0"/>
         <v>0.39999999999999858</v>
       </c>
       <c r="M2">
-        <f xml:space="preserve"> G2 - ABS(D2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3920,15 +3952,15 @@
         <v>39</v>
       </c>
       <c r="K3">
-        <f xml:space="preserve"> E3 - ABS(B3)</f>
+        <f t="shared" si="0"/>
         <v>0.89999999999999858</v>
       </c>
       <c r="L3">
-        <f xml:space="preserve"> F3 - ABS(C3)</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="M3">
-        <f xml:space="preserve"> G3 - ABS(D3)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3949,15 +3981,15 @@
         <v>38.5</v>
       </c>
       <c r="K4">
-        <f xml:space="preserve"> E4 - ABS(B4)</f>
+        <f t="shared" si="0"/>
         <v>1.2999999999999972</v>
       </c>
       <c r="L4">
-        <f xml:space="preserve"> F4 - ABS(C4)</f>
+        <f t="shared" si="0"/>
         <v>0.70000000000000284</v>
       </c>
       <c r="M4">
-        <f xml:space="preserve"> G4 - ABS(D4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3978,15 +4010,15 @@
         <v>8</v>
       </c>
       <c r="K7">
-        <f t="shared" ref="K5:K8" si="0" xml:space="preserve"> E7 - ABS(B7)</f>
+        <f t="shared" ref="K7:K8" si="1" xml:space="preserve"> E7 - ABS(B7)</f>
         <v>-0.1</v>
       </c>
       <c r="L7">
-        <f t="shared" ref="L5:L8" si="1" xml:space="preserve"> F7 - ABS(C7)</f>
+        <f t="shared" ref="L7:L8" si="2" xml:space="preserve"> F7 - ABS(C7)</f>
         <v>-0.69999999999999929</v>
       </c>
       <c r="M7">
-        <f t="shared" ref="M5:M8" si="2" xml:space="preserve"> G7 - ABS(D7)</f>
+        <f t="shared" ref="M7:M8" si="3" xml:space="preserve"> G7 - ABS(D7)</f>
         <v>0</v>
       </c>
     </row>
@@ -4007,15 +4039,15 @@
         <v>14</v>
       </c>
       <c r="K8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.1</v>
       </c>
       <c r="L8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.80000000000000071</v>
       </c>
       <c r="M8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -4036,15 +4068,15 @@
         <v>24</v>
       </c>
       <c r="K9">
-        <f t="shared" ref="K9" si="3" xml:space="preserve"> E9 - ABS(B9)</f>
+        <f t="shared" ref="K9" si="4" xml:space="preserve"> E9 - ABS(B9)</f>
         <v>0</v>
       </c>
       <c r="L9">
-        <f t="shared" ref="L9" si="4" xml:space="preserve"> F9 - ABS(C9)</f>
+        <f t="shared" ref="L9" si="5" xml:space="preserve"> F9 - ABS(C9)</f>
         <v>-0.89999999999999858</v>
       </c>
       <c r="M9">
-        <f t="shared" ref="M9" si="5" xml:space="preserve"> G9 - ABS(D9)</f>
+        <f t="shared" ref="M9" si="6" xml:space="preserve"> G9 - ABS(D9)</f>
         <v>0</v>
       </c>
     </row>
@@ -4065,15 +4097,15 @@
         <v>8.25</v>
       </c>
       <c r="K10">
-        <f t="shared" ref="K10:K11" si="6" xml:space="preserve"> E10 - ABS(B10)</f>
+        <f t="shared" ref="K10:K11" si="7" xml:space="preserve"> E10 - ABS(B10)</f>
         <v>-0.1</v>
       </c>
       <c r="L10">
-        <f t="shared" ref="L10:L11" si="7" xml:space="preserve"> F10 - ABS(C10)</f>
+        <f t="shared" ref="L10:L11" si="8" xml:space="preserve"> F10 - ABS(C10)</f>
         <v>-0.55000000000000071</v>
       </c>
       <c r="M10">
-        <f t="shared" ref="M10" si="8" xml:space="preserve"> G10 - ABS(D10)</f>
+        <f t="shared" ref="M10" si="9" xml:space="preserve"> G10 - ABS(D10)</f>
         <v>0</v>
       </c>
     </row>
@@ -4094,11 +4126,11 @@
         <v>14.25</v>
       </c>
       <c r="K11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-0.3</v>
       </c>
       <c r="L11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-0.65000000000000036</v>
       </c>
     </row>
@@ -4119,11 +4151,11 @@
         <v>24.5</v>
       </c>
       <c r="K12">
-        <f t="shared" ref="K12" si="9" xml:space="preserve"> E12 - ABS(B12)</f>
+        <f t="shared" ref="K12" si="10" xml:space="preserve"> E12 - ABS(B12)</f>
         <v>-0.6</v>
       </c>
       <c r="L12">
-        <f t="shared" ref="L12" si="10" xml:space="preserve"> F12 - ABS(C12)</f>
+        <f t="shared" ref="L12" si="11" xml:space="preserve"> F12 - ABS(C12)</f>
         <v>-0.5</v>
       </c>
     </row>
@@ -4144,11 +4176,11 @@
         <v>8</v>
       </c>
       <c r="K13">
-        <f t="shared" ref="K13" si="11" xml:space="preserve"> E13 - ABS(B13)</f>
+        <f t="shared" ref="K13" si="12" xml:space="preserve"> E13 - ABS(B13)</f>
         <v>0</v>
       </c>
       <c r="L13">
-        <f t="shared" ref="L13" si="12" xml:space="preserve"> F13 - ABS(C13)</f>
+        <f t="shared" ref="L13" si="13" xml:space="preserve"> F13 - ABS(C13)</f>
         <v>-1</v>
       </c>
     </row>
@@ -4191,7 +4223,7 @@
     </row>
     <row r="23" spans="12:13">
       <c r="L23">
-        <f t="shared" ref="L23:L32" si="13">L3-$M$20</f>
+        <f t="shared" ref="L23:L32" si="14">L3-$M$20</f>
         <v>0.84999999999999987</v>
       </c>
     </row>
@@ -4209,35 +4241,476 @@
     </row>
     <row r="28" spans="12:13">
       <c r="L28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-0.4500000000000009</v>
       </c>
     </row>
     <row r="29" spans="12:13">
       <c r="L29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-0.54999999999999871</v>
       </c>
     </row>
     <row r="30" spans="12:13">
       <c r="L30">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-0.2000000000000009</v>
       </c>
     </row>
     <row r="31" spans="12:13">
       <c r="L31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-0.30000000000000054</v>
       </c>
     </row>
     <row r="32" spans="12:13">
       <c r="L32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-0.15000000000000019</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5877923-39D9-144B-B71F-E88B807B65F3}">
+  <dimension ref="A1:M34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="1">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-38.6</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1">
+        <v>34.9</v>
+      </c>
+      <c r="F2" s="1">
+        <v>55.5</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ref="K2:M2" si="0" xml:space="preserve"> E2 - ABS(B2)</f>
+        <v>7.8999999999999986</v>
+      </c>
+      <c r="L2">
+        <f xml:space="preserve"> F2 - ABS(C2)</f>
+        <v>16.899999999999999</v>
+      </c>
+      <c r="M2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-35.299999999999997</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-56.8</v>
+      </c>
+      <c r="E3">
+        <v>35.5</v>
+      </c>
+      <c r="F3">
+        <v>57</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3" si="1" xml:space="preserve"> E3 - ABS(B3)</f>
+        <v>0.20000000000000284</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3" si="2" xml:space="preserve"> F3 - ABS(C3)</f>
+        <v>0.20000000000000284</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3" si="3" xml:space="preserve"> G3 - ABS(D3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="1">
+        <v>35.6</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-51.4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>35.5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>55.5</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ref="K5:K6" si="4" xml:space="preserve"> E5 - ABS(B5)</f>
+        <v>-0.10000000000000142</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5:L6" si="5" xml:space="preserve"> F5 - ABS(C5)</f>
+        <v>4.1000000000000014</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M6" si="6" xml:space="preserve"> G5 - ABS(D5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="1">
+        <v>29.6</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-51.6</v>
+      </c>
+      <c r="E6">
+        <v>29.5</v>
+      </c>
+      <c r="F6">
+        <v>55.5</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="4"/>
+        <v>-0.10000000000000142</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="5"/>
+        <v>3.8999999999999986</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="1">
+        <v>41.5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-51.5</v>
+      </c>
+      <c r="E7">
+        <v>41.5</v>
+      </c>
+      <c r="F7">
+        <v>55.5</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ref="K7" si="7" xml:space="preserve"> E7 - ABS(B7)</f>
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <f t="shared" ref="L7" si="8" xml:space="preserve"> F7 - ABS(C7)</f>
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <f t="shared" ref="M7" si="9" xml:space="preserve"> G7 - ABS(D7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="1">
+        <v>29.7</v>
+      </c>
+      <c r="C9" s="1">
+        <v>-45.2</v>
+      </c>
+      <c r="E9">
+        <v>29.5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>48.5</v>
+      </c>
+      <c r="K9">
+        <f xml:space="preserve"> E9 - ABS(B9)</f>
+        <v>-0.19999999999999929</v>
+      </c>
+      <c r="L9">
+        <f t="shared" ref="L8:L11" si="10" xml:space="preserve"> F9 - ABS(C9)</f>
+        <v>3.2999999999999972</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ref="M8:M11" si="11" xml:space="preserve"> G9 - ABS(D9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="1">
+        <v>35.6</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-45.3</v>
+      </c>
+      <c r="E10">
+        <v>35.5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>48.5</v>
+      </c>
+      <c r="K10">
+        <f xml:space="preserve"> E10 - ABS(B10)</f>
+        <v>-0.10000000000000142</v>
+      </c>
+      <c r="L10">
+        <f xml:space="preserve"> F10 - ABS(C10)</f>
+        <v>3.2000000000000028</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="1">
+        <v>41.3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>-45.5</v>
+      </c>
+      <c r="E11">
+        <v>41.5</v>
+      </c>
+      <c r="F11" s="6">
+        <v>48.5</v>
+      </c>
+      <c r="K11">
+        <f xml:space="preserve"> E11 - ABS(B11)</f>
+        <v>0.20000000000000284</v>
+      </c>
+      <c r="L11">
+        <f xml:space="preserve"> F11 - ABS(C11)</f>
+        <v>3</v>
+      </c>
+      <c r="M11">
+        <f t="shared" ref="M11" si="12" xml:space="preserve"> G11 - ABS(D11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="1">
+        <v>41.5</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-35.4</v>
+      </c>
+      <c r="E13">
+        <v>41.5</v>
+      </c>
+      <c r="F13">
+        <v>38.5</v>
+      </c>
+      <c r="K13">
+        <f t="shared" ref="K12:K15" si="13" xml:space="preserve"> E13 - ABS(B13)</f>
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f t="shared" ref="L12:L15" si="14" xml:space="preserve"> F13 - ABS(C13)</f>
+        <v>3.1000000000000014</v>
+      </c>
+      <c r="M13">
+        <f t="shared" ref="M12:M15" si="15" xml:space="preserve"> G13 - ABS(D13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="1">
+        <v>35.1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-35.299999999999997</v>
+      </c>
+      <c r="E14">
+        <v>35.5</v>
+      </c>
+      <c r="F14">
+        <v>38.5</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="13"/>
+        <v>0.39999999999999858</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="14"/>
+        <v>3.2000000000000028</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="1">
+        <v>29.4</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-35.200000000000003</v>
+      </c>
+      <c r="E15">
+        <v>29.5</v>
+      </c>
+      <c r="F15">
+        <v>38.5</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="13"/>
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="14"/>
+        <v>3.2999999999999972</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="11:12">
+      <c r="K17" t="s">
+        <v>105</v>
+      </c>
+      <c r="L17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="11:12">
+      <c r="L18" s="7">
+        <f>AVERAGE(L5:L7,L9:L11,L13:L15)</f>
+        <v>3.4555555555555557</v>
+      </c>
+    </row>
+    <row r="20" spans="11:12">
+      <c r="L20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="11:12">
+      <c r="L22">
+        <f>L5-$L$18</f>
+        <v>0.64444444444444571</v>
+      </c>
+    </row>
+    <row r="23" spans="11:12">
+      <c r="L23">
+        <f>L6-$L$18</f>
+        <v>0.44444444444444287</v>
+      </c>
+    </row>
+    <row r="24" spans="11:12">
+      <c r="L24">
+        <f>L7-$L$18</f>
+        <v>0.54444444444444429</v>
+      </c>
+    </row>
+    <row r="26" spans="11:12">
+      <c r="L26">
+        <f t="shared" ref="L24:L33" si="16">L9-$L$18</f>
+        <v>-0.15555555555555856</v>
+      </c>
+    </row>
+    <row r="27" spans="11:12">
+      <c r="L27">
+        <f t="shared" si="16"/>
+        <v>-0.25555555555555287</v>
+      </c>
+    </row>
+    <row r="28" spans="11:12">
+      <c r="L28">
+        <f t="shared" si="16"/>
+        <v>-0.45555555555555571</v>
+      </c>
+    </row>
+    <row r="30" spans="11:12">
+      <c r="L30">
+        <f>L13-$L$18</f>
+        <v>-0.35555555555555429</v>
+      </c>
+    </row>
+    <row r="31" spans="11:12">
+      <c r="L31">
+        <f t="shared" si="16"/>
+        <v>-0.25555555555555287</v>
+      </c>
+    </row>
+    <row r="32" spans="11:12">
+      <c r="L32">
+        <f t="shared" si="16"/>
+        <v>-0.15555555555555856</v>
+      </c>
+    </row>
+    <row r="34" spans="12:12">
+      <c r="L34">
+        <f>8.125-7.7</f>
+        <v>0.42499999999999982</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Proves that apriltag calibration is possible with 4 points-yay\!
</commit_message>
<xml_diff>
--- a/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
+++ b/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/Dropbox/Brain Stormz FTC/2023-24-code/AprilTag Performance Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EFADD4-A4E3-0249-9F25-B2ACE35EBC5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146CBFA6-266B-FB4D-A1C4-5B11DD4CAA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="6" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="7" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="Worlds-like test" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="114">
   <si>
     <t>Point</t>
   </si>
@@ -363,13 +364,34 @@
   </si>
   <si>
     <t>ADJUSTED Y</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>AVG X ERR</t>
+  </si>
+  <si>
+    <t>PROCESSED</t>
+  </si>
+  <si>
+    <t>SPIKE (B5) - important point</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -402,13 +424,31 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -423,17 +463,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4278,8 +4321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5877923-39D9-144B-B71F-E88B807B65F3}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4477,11 +4520,11 @@
         <v>-0.19999999999999929</v>
       </c>
       <c r="L9">
-        <f t="shared" ref="L8:L11" si="10" xml:space="preserve"> F9 - ABS(C9)</f>
+        <f t="shared" ref="L9" si="10" xml:space="preserve"> F9 - ABS(C9)</f>
         <v>3.2999999999999972</v>
       </c>
       <c r="M9">
-        <f t="shared" ref="M8:M11" si="11" xml:space="preserve"> G9 - ABS(D9)</f>
+        <f t="shared" ref="M9:M10" si="11" xml:space="preserve"> G9 - ABS(D9)</f>
         <v>0</v>
       </c>
     </row>
@@ -4560,15 +4603,15 @@
         <v>38.5</v>
       </c>
       <c r="K13">
-        <f t="shared" ref="K12:K15" si="13" xml:space="preserve"> E13 - ABS(B13)</f>
+        <f t="shared" ref="K13:K15" si="13" xml:space="preserve"> E13 - ABS(B13)</f>
         <v>0</v>
       </c>
       <c r="L13">
-        <f t="shared" ref="L12:L15" si="14" xml:space="preserve"> F13 - ABS(C13)</f>
+        <f t="shared" ref="L13:L15" si="14" xml:space="preserve"> F13 - ABS(C13)</f>
         <v>3.1000000000000014</v>
       </c>
       <c r="M13">
-        <f t="shared" ref="M12:M15" si="15" xml:space="preserve"> G13 - ABS(D13)</f>
+        <f t="shared" ref="M13:M15" si="15" xml:space="preserve"> G13 - ABS(D13)</f>
         <v>0</v>
       </c>
     </row>
@@ -4669,7 +4712,7 @@
     </row>
     <row r="26" spans="11:12">
       <c r="L26">
-        <f t="shared" ref="L24:L33" si="16">L9-$L$18</f>
+        <f t="shared" ref="L26:L32" si="16">L9-$L$18</f>
         <v>-0.15555555555555856</v>
       </c>
     </row>
@@ -4707,6 +4750,338 @@
       <c r="L34">
         <f>8.125-7.7</f>
         <v>0.42499999999999982</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2014BCED-35E7-FE44-9FDA-065FB736E196}">
+  <dimension ref="A1:M28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="1">
+        <v>48</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-44</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="10">
+        <v>47.5</v>
+      </c>
+      <c r="F2" s="10">
+        <v>47.625</v>
+      </c>
+      <c r="K2">
+        <f xml:space="preserve"> E2 - ABS(B2)</f>
+        <v>-0.5</v>
+      </c>
+      <c r="L2">
+        <f xml:space="preserve"> F2 - ABS(C2)</f>
+        <v>3.625</v>
+      </c>
+      <c r="M2">
+        <f t="shared" ref="K2:M2" si="0" xml:space="preserve"> G2 - ABS(D2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="1">
+        <v>23.7</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-44.5</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="10">
+        <v>23.625</v>
+      </c>
+      <c r="F3" s="10">
+        <v>47.625</v>
+      </c>
+      <c r="H3">
+        <f>5/8</f>
+        <v>0.625</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K5" si="1" xml:space="preserve"> E3 - ABS(B3)</f>
+        <v>-7.4999999999999289E-2</v>
+      </c>
+      <c r="L3">
+        <f xml:space="preserve"> F3 - ABS(C3)</f>
+        <v>3.125</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M6" si="2" xml:space="preserve"> G3 - ABS(D3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="1">
+        <v>47.4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-19.899999999999999</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="10">
+        <v>47.5</v>
+      </c>
+      <c r="F4" s="10">
+        <v>23.875</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L3:L6" si="3" xml:space="preserve"> F4 - ABS(C4)</f>
+        <v>3.9750000000000014</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="1">
+        <v>23.6</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-20.3</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="10">
+        <v>23.75</v>
+      </c>
+      <c r="F5" s="10">
+        <v>23.875</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>0.14999999999999858</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="3"/>
+        <v>3.5749999999999993</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="9">
+        <v>-1.8</v>
+      </c>
+      <c r="C6" s="9">
+        <v>-21.3</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9">
+        <v>0</v>
+      </c>
+      <c r="F6" s="9">
+        <v>23.75</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8">
+        <f t="shared" ref="K3:K6" si="4" xml:space="preserve"> E6 - ABS(B6)</f>
+        <v>-1.8</v>
+      </c>
+      <c r="L6" s="8">
+        <f t="shared" si="3"/>
+        <v>2.4499999999999993</v>
+      </c>
+      <c r="M6" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="1">
+        <v>14.4</v>
+      </c>
+      <c r="C8" s="1">
+        <v>-20.6</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1">
+        <v>15.625</v>
+      </c>
+      <c r="F8" s="1">
+        <v>23.375</v>
+      </c>
+      <c r="K8" s="8">
+        <f xml:space="preserve"> E8 - ABS(B8)</f>
+        <v>1.2249999999999996</v>
+      </c>
+      <c r="L8" s="8">
+        <f xml:space="preserve"> F8 - ABS(C8)</f>
+        <v>2.7749999999999986</v>
+      </c>
+      <c r="M8" s="8">
+        <f t="shared" ref="M7:M8" si="5" xml:space="preserve"> G8 - ABS(D8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="K10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="K12">
+        <f>K8-K23</f>
+        <v>1.0449999999999995</v>
+      </c>
+      <c r="L12">
+        <f>L8-L23</f>
+        <v>-0.64000000000000146</v>
+      </c>
+    </row>
+    <row r="22" spans="11:12">
+      <c r="K22" t="s">
+        <v>111</v>
+      </c>
+      <c r="L22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="11:12">
+      <c r="K23">
+        <f>AVERAGE(K2:K5, K8)</f>
+        <v>0.18000000000000008</v>
+      </c>
+      <c r="L23">
+        <f>AVERAGE(L2:L5, L8)</f>
+        <v>3.415</v>
+      </c>
+    </row>
+    <row r="25" spans="11:12">
+      <c r="K25">
+        <f>K2-$K$23</f>
+        <v>-0.68</v>
+      </c>
+      <c r="L25">
+        <f>L2-$L$23</f>
+        <v>0.20999999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="11:12">
+      <c r="K26">
+        <f>K3-$K$23</f>
+        <v>-0.25499999999999934</v>
+      </c>
+      <c r="L26">
+        <f>L3-$L$23</f>
+        <v>-0.29000000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="11:12">
+      <c r="K27">
+        <f>K4-$K$23</f>
+        <v>-7.9999999999998656E-2</v>
+      </c>
+      <c r="L27">
+        <f>L4-$L$23</f>
+        <v>0.56000000000000139</v>
+      </c>
+    </row>
+    <row r="28" spans="11:12">
+      <c r="K28">
+        <f>K5-$K$23</f>
+        <v>-3.0000000000001498E-2</v>
+      </c>
+      <c r="L28">
+        <f>L5-$L$23</f>
+        <v>0.15999999999999925</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial values of apriltag test coordinates
</commit_message>
<xml_diff>
--- a/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
+++ b/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/Dropbox/Brain Stormz FTC/2023-24-code/AprilTag Performance Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146CBFA6-266B-FB4D-A1C4-5B11DD4CAA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686A5225-32B9-2748-8FF2-53ADBFBD12DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="7" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="118">
   <si>
     <t>Point</t>
   </si>
@@ -385,13 +385,25 @@
   </si>
   <si>
     <t>SPIKE (B5) - important point</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -430,6 +442,12 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -463,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -477,6 +495,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4760,10 +4779,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2014BCED-35E7-FE44-9FDA-065FB736E196}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5018,71 +5037,212 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="K12">
-        <f>K8-K23</f>
+        <f>K8-K18</f>
         <v>1.0449999999999995</v>
       </c>
       <c r="L12">
-        <f>L8-L23</f>
+        <f>L8-L18</f>
         <v>-0.64000000000000146</v>
       </c>
     </row>
-    <row r="22" spans="11:12">
-      <c r="K22" t="s">
+    <row r="17" spans="1:13">
+      <c r="K17" t="s">
         <v>111</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L17" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="11:12">
-      <c r="K23">
+    <row r="18" spans="1:13">
+      <c r="K18">
         <f>AVERAGE(K2:K5, K8)</f>
         <v>0.18000000000000008</v>
       </c>
-      <c r="L23">
+      <c r="L18">
         <f>AVERAGE(L2:L5, L8)</f>
         <v>3.415</v>
       </c>
     </row>
-    <row r="25" spans="11:12">
-      <c r="K25">
-        <f>K2-$K$23</f>
+    <row r="20" spans="1:13">
+      <c r="K20">
+        <f>K2-$K$18</f>
         <v>-0.68</v>
       </c>
-      <c r="L25">
-        <f>L2-$L$23</f>
+      <c r="L20">
+        <f>L2-$L$18</f>
         <v>0.20999999999999996</v>
       </c>
     </row>
-    <row r="26" spans="11:12">
-      <c r="K26">
-        <f>K3-$K$23</f>
+    <row r="21" spans="1:13">
+      <c r="K21">
+        <f>K3-$K$18</f>
         <v>-0.25499999999999934</v>
       </c>
-      <c r="L26">
-        <f>L3-$L$23</f>
+      <c r="L21">
+        <f>L3-$L$18</f>
         <v>-0.29000000000000004</v>
       </c>
     </row>
-    <row r="27" spans="11:12">
-      <c r="K27">
-        <f>K4-$K$23</f>
+    <row r="22" spans="1:13">
+      <c r="K22">
+        <f>K4-$K$18</f>
         <v>-7.9999999999998656E-2</v>
       </c>
-      <c r="L27">
-        <f>L4-$L$23</f>
+      <c r="L22">
+        <f>L4-$L$18</f>
         <v>0.56000000000000139</v>
       </c>
     </row>
-    <row r="28" spans="11:12">
-      <c r="K28">
-        <f>K5-$K$23</f>
+    <row r="23" spans="1:13">
+      <c r="K23">
+        <f>K5-$K$18</f>
         <v>-3.0000000000001498E-2</v>
       </c>
-      <c r="L28">
-        <f>L5-$L$23</f>
+      <c r="L23">
+        <f>L5-$L$18</f>
         <v>0.15999999999999925</v>
       </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="H29">
+        <f>3/8</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" s="1">
+        <v>48</v>
+      </c>
+      <c r="C30" s="1">
+        <v>-44</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="11">
+        <v>23.875</v>
+      </c>
+      <c r="F30" s="11">
+        <v>47.625</v>
+      </c>
+      <c r="K30">
+        <f xml:space="preserve"> E30 - ABS(B30)</f>
+        <v>-24.125</v>
+      </c>
+      <c r="L30">
+        <f xml:space="preserve"> F30 - ABS(C30)</f>
+        <v>3.625</v>
+      </c>
+      <c r="M30">
+        <f t="shared" ref="M30:M34" si="6" xml:space="preserve"> G30 - ABS(D30)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="1">
+        <v>23.7</v>
+      </c>
+      <c r="C31" s="1">
+        <v>-44.5</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="11">
+        <v>47.625</v>
+      </c>
+      <c r="F31" s="11">
+        <v>47.625</v>
+      </c>
+      <c r="K31">
+        <f t="shared" ref="K31:K34" si="7" xml:space="preserve"> E31 - ABS(B31)</f>
+        <v>23.925000000000001</v>
+      </c>
+      <c r="L31">
+        <f xml:space="preserve"> F31 - ABS(C31)</f>
+        <v>3.125</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" s="1">
+        <v>47.4</v>
+      </c>
+      <c r="C32" s="1">
+        <v>-19.899999999999999</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="11">
+        <v>23.875</v>
+      </c>
+      <c r="F32" s="11">
+        <v>23.375</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="7"/>
+        <v>-23.524999999999999</v>
+      </c>
+      <c r="L32">
+        <f t="shared" ref="L32:L34" si="8" xml:space="preserve"> F32 - ABS(C32)</f>
+        <v>3.4750000000000014</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" t="s">
+        <v>117</v>
+      </c>
+      <c r="B33" s="1">
+        <v>23.6</v>
+      </c>
+      <c r="C33" s="1">
+        <v>-20.3</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="11">
+        <v>47.625</v>
+      </c>
+      <c r="F33" s="11">
+        <v>23.375</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="7"/>
+        <v>24.024999999999999</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="8"/>
+        <v>3.0749999999999993</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="8"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Removes all anti-null proceedures from AprilTag.
</commit_message>
<xml_diff>
--- a/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
+++ b/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/Dropbox/Brain Stormz FTC/2023-24-code/AprilTag Performance Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4274FC5D-C0C8-EF45-A9A6-67FACAF8C7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EE89B7-3EF2-3A42-B2C6-69F1C242BF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="7" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
+    <workbookView xWindow="-800" yWindow="2080" windowWidth="28800" windowHeight="14660" activeTab="8" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,10 @@
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
     <sheet name="Worlds-like test" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet8" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -501,7 +503,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4787,8 +4789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2014BCED-35E7-FE44-9FDA-065FB736E196}">
   <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="83" workbookViewId="0">
-      <selection activeCell="L55" sqref="L55"/>
+    <sheetView topLeftCell="A8" zoomScale="83" workbookViewId="0">
+      <selection sqref="A1:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4845,7 +4847,7 @@
         <v>3.625</v>
       </c>
       <c r="M2">
-        <f t="shared" ref="K2:M2" si="0" xml:space="preserve"> G2 - ABS(D2)</f>
+        <f t="shared" ref="M2" si="0" xml:space="preserve"> G2 - ABS(D2)</f>
         <v>0</v>
       </c>
     </row>
@@ -4871,7 +4873,7 @@
         <v>0.625</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K5" si="1" xml:space="preserve"> E3 - ABS(B3)</f>
+        <f xml:space="preserve"> E3 - ABS(B3)</f>
         <v>-7.4999999999999289E-2</v>
       </c>
       <c r="L3">
@@ -4879,7 +4881,7 @@
         <v>3.125</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M6" si="2" xml:space="preserve"> G3 - ABS(D3)</f>
+        <f t="shared" ref="M3:M6" si="1" xml:space="preserve"> G3 - ABS(D3)</f>
         <v>0</v>
       </c>
     </row>
@@ -4901,15 +4903,15 @@
         <v>23.875</v>
       </c>
       <c r="K4">
+        <f xml:space="preserve"> E4 - ABS(B4)</f>
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="L4">
+        <f xml:space="preserve"> F4 - ABS(C4)</f>
+        <v>3.9750000000000014</v>
+      </c>
+      <c r="M4">
         <f t="shared" si="1"/>
-        <v>0.10000000000000142</v>
-      </c>
-      <c r="L4">
-        <f t="shared" ref="L3:L6" si="3" xml:space="preserve"> F4 - ABS(C4)</f>
-        <v>3.9750000000000014</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4931,15 +4933,15 @@
         <v>23.875</v>
       </c>
       <c r="K5">
+        <f xml:space="preserve"> E5 - ABS(B5)</f>
+        <v>0.14999999999999858</v>
+      </c>
+      <c r="L5">
+        <f xml:space="preserve"> F5 - ABS(C5)</f>
+        <v>3.5749999999999993</v>
+      </c>
+      <c r="M5">
         <f t="shared" si="1"/>
-        <v>0.14999999999999858</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="3"/>
-        <v>3.5749999999999993</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -4965,15 +4967,15 @@
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8">
-        <f t="shared" ref="K6" si="4" xml:space="preserve"> E6 - ABS(B6)</f>
+        <f t="shared" ref="K6" si="2" xml:space="preserve"> E6 - ABS(B6)</f>
         <v>-1.8</v>
       </c>
       <c r="L6" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="L4:L6" si="3" xml:space="preserve"> F6 - ABS(C6)</f>
         <v>2.4499999999999993</v>
       </c>
       <c r="M6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5008,7 +5010,7 @@
         <v>2.7749999999999986</v>
       </c>
       <c r="M8" s="8">
-        <f t="shared" ref="M8" si="5" xml:space="preserve"> G8 - ABS(D8)</f>
+        <f t="shared" ref="M8" si="4" xml:space="preserve"> G8 - ABS(D8)</f>
         <v>0</v>
       </c>
     </row>
@@ -5070,7 +5072,7 @@
         <v>2.4999999999998579E-2</v>
       </c>
       <c r="M13">
-        <f t="shared" ref="M13" si="6" xml:space="preserve"> G13 - ABS(D13)</f>
+        <f t="shared" ref="M13" si="5" xml:space="preserve"> G13 - ABS(D13)</f>
         <v>0</v>
       </c>
     </row>
@@ -5092,7 +5094,7 @@
         <v>47.625</v>
       </c>
       <c r="K15">
-        <f t="shared" ref="K15" si="7" xml:space="preserve"> E15 - ABS(B15)</f>
+        <f t="shared" ref="K15" si="6" xml:space="preserve"> E15 - ABS(B15)</f>
         <v>0.42499999999999716</v>
       </c>
       <c r="L15">
@@ -5100,7 +5102,7 @@
         <v>-0.17499999999999716</v>
       </c>
       <c r="M15">
-        <f t="shared" ref="M15" si="8" xml:space="preserve"> G15 - ABS(D15)</f>
+        <f t="shared" ref="M15" si="7" xml:space="preserve"> G15 - ABS(D15)</f>
         <v>0</v>
       </c>
     </row>
@@ -5202,7 +5204,7 @@
         <v>3.4249999999999972</v>
       </c>
       <c r="M30">
-        <f t="shared" ref="M30:M33" si="9" xml:space="preserve"> G30 - ABS(D30)</f>
+        <f t="shared" ref="M30:M33" si="8" xml:space="preserve"> G30 - ABS(D30)</f>
         <v>0</v>
       </c>
     </row>
@@ -5224,7 +5226,7 @@
         <v>47.625</v>
       </c>
       <c r="K31">
-        <f t="shared" ref="K31" si="10" xml:space="preserve"> E31 - ABS(B31)</f>
+        <f t="shared" ref="K31" si="9" xml:space="preserve"> E31 - ABS(B31)</f>
         <v>0.125</v>
       </c>
       <c r="L31">
@@ -5232,7 +5234,7 @@
         <v>3.0249999999999986</v>
       </c>
       <c r="M31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -5258,11 +5260,11 @@
         <v>-0.82499999999999929</v>
       </c>
       <c r="L32">
-        <f t="shared" ref="L32" si="11" xml:space="preserve"> F32 - ABS(C32)</f>
+        <f t="shared" ref="L32" si="10" xml:space="preserve"> F32 - ABS(C32)</f>
         <v>3.5749999999999993</v>
       </c>
       <c r="M32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -5292,7 +5294,7 @@
         <v>2.5749999999999993</v>
       </c>
       <c r="M33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -5325,15 +5327,15 @@
         <v>40.5</v>
       </c>
       <c r="K36">
-        <f t="shared" ref="K34:K36" si="12" xml:space="preserve"> E36 - ABS(B36)</f>
+        <f t="shared" ref="K36" si="11" xml:space="preserve"> E36 - ABS(B36)</f>
         <v>0.60000000000000142</v>
       </c>
       <c r="L36">
-        <f t="shared" ref="L34:L36" si="13" xml:space="preserve"> F36 - ABS(C36)</f>
+        <f t="shared" ref="L36" si="12" xml:space="preserve"> F36 - ABS(C36)</f>
         <v>-9.1000000000000014</v>
       </c>
       <c r="M36">
-        <f t="shared" ref="M34:M36" si="14" xml:space="preserve"> G36 - ABS(D36)</f>
+        <f t="shared" ref="M36" si="13" xml:space="preserve"> G36 - ABS(D36)</f>
         <v>0</v>
       </c>
     </row>
@@ -5382,31 +5384,31 @@
     </row>
     <row r="49" spans="11:12">
       <c r="K49">
-        <f t="shared" ref="K49:K51" si="15">K31-$K$20</f>
+        <f t="shared" ref="K49:K51" si="14">K31-$K$20</f>
         <v>0.20624999999999982</v>
       </c>
       <c r="L49">
-        <f t="shared" ref="L49:L51" si="16">L31-$L$46</f>
+        <f t="shared" ref="L49:L51" si="15">L31-$L$46</f>
         <v>-0.125</v>
       </c>
     </row>
     <row r="50" spans="11:12">
       <c r="K50">
+        <f t="shared" si="14"/>
+        <v>-0.74374999999999947</v>
+      </c>
+      <c r="L50">
         <f t="shared" si="15"/>
-        <v>-0.74374999999999947</v>
-      </c>
-      <c r="L50">
-        <f t="shared" si="16"/>
         <v>0.42500000000000071</v>
       </c>
     </row>
     <row r="51" spans="11:12">
       <c r="K51">
+        <f t="shared" si="14"/>
+        <v>-0.8937500000000016</v>
+      </c>
+      <c r="L51">
         <f t="shared" si="15"/>
-        <v>-0.8937500000000016</v>
-      </c>
-      <c r="L51">
-        <f t="shared" si="16"/>
         <v>-0.57499999999999929</v>
       </c>
     </row>
@@ -5427,21 +5429,21 @@
     </row>
     <row r="56" spans="11:12">
       <c r="K56">
-        <f t="shared" ref="K56:K58" si="17">K31-$K$20</f>
+        <f t="shared" ref="K56:K57" si="16">K31-$K$20</f>
         <v>0.20624999999999982</v>
       </c>
       <c r="L56">
-        <f t="shared" ref="L56:L58" si="18">L38-$L$46</f>
+        <f t="shared" ref="L56:L58" si="17">L38-$L$46</f>
         <v>-3.1499999999999986</v>
       </c>
     </row>
     <row r="57" spans="11:12">
       <c r="K57">
+        <f t="shared" si="16"/>
+        <v>-0.74374999999999947</v>
+      </c>
+      <c r="L57">
         <f t="shared" si="17"/>
-        <v>-0.74374999999999947</v>
-      </c>
-      <c r="L57">
-        <f t="shared" si="18"/>
         <v>-15.824999999999999</v>
       </c>
     </row>
@@ -5451,7 +5453,7 @@
         <v>-0.8937500000000016</v>
       </c>
       <c r="L58">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>-3.1499999999999986</v>
       </c>
     </row>
@@ -5459,4 +5461,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{844DCAFA-79F0-1F49-AC05-9154084A1CAD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adds easy 0 offset for AprilTag
</commit_message>
<xml_diff>
--- a/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
+++ b/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/Dropbox/Brain Stormz FTC/2023-24-code/AprilTag Performance Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EE89B7-3EF2-3A42-B2C6-69F1C242BF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CE9AD0-AAB7-944E-BA9F-3ECD893E4A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-800" yWindow="2080" windowWidth="28800" windowHeight="14660" activeTab="8" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
+    <workbookView xWindow="560" yWindow="2080" windowWidth="28800" windowHeight="14660" activeTab="7" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
     <sheet name="Worlds-like test" sheetId="8" r:id="rId8"/>
-    <sheet name="Sheet8" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -4789,7 +4788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2014BCED-35E7-FE44-9FDA-065FB736E196}">
   <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="83" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="83" workbookViewId="0">
       <selection sqref="A1:M5"/>
     </sheetView>
   </sheetViews>
@@ -5461,16 +5460,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{844DCAFA-79F0-1F49-AC05-9154084A1CAD}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
adds average error library to AprilTag
</commit_message>
<xml_diff>
--- a/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
+++ b/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/Dropbox/Brain Stormz FTC/2023-24-code/AprilTag Performance Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CE9AD0-AAB7-944E-BA9F-3ECD893E4A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC98E399-4F9F-914F-A279-F0D0F5DE234E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="2080" windowWidth="28800" windowHeight="14660" activeTab="7" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
+    <workbookView xWindow="400" yWindow="3940" windowWidth="28800" windowHeight="14660" activeTab="7" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4788,8 +4788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2014BCED-35E7-FE44-9FDA-065FB736E196}">
   <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="83" workbookViewId="0">
-      <selection sqref="A1:M5"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4855,10 +4855,10 @@
         <v>28</v>
       </c>
       <c r="B3" s="1">
-        <v>23.7</v>
+        <v>23.5</v>
       </c>
       <c r="C3" s="1">
-        <v>-44.5</v>
+        <v>-44.2</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="10">
@@ -4873,11 +4873,11 @@
       </c>
       <c r="K3">
         <f xml:space="preserve"> E3 - ABS(B3)</f>
-        <v>-7.4999999999999289E-2</v>
+        <v>0.125</v>
       </c>
       <c r="L3">
         <f xml:space="preserve"> F3 - ABS(C3)</f>
-        <v>3.125</v>
+        <v>3.4249999999999972</v>
       </c>
       <c r="M3">
         <f t="shared" ref="M3:M6" si="1" xml:space="preserve"> G3 - ABS(D3)</f>
@@ -4889,10 +4889,10 @@
         <v>108</v>
       </c>
       <c r="B4" s="1">
-        <v>47.4</v>
+        <v>47.1</v>
       </c>
       <c r="C4" s="1">
-        <v>-19.899999999999999</v>
+        <v>-20.100000000000001</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="10">
@@ -4903,11 +4903,11 @@
       </c>
       <c r="K4">
         <f xml:space="preserve"> E4 - ABS(B4)</f>
-        <v>0.10000000000000142</v>
+        <v>0.39999999999999858</v>
       </c>
       <c r="L4">
         <f xml:space="preserve"> F4 - ABS(C4)</f>
-        <v>3.9750000000000014</v>
+        <v>3.7749999999999986</v>
       </c>
       <c r="M4">
         <f t="shared" si="1"/>
@@ -4922,7 +4922,7 @@
         <v>23.6</v>
       </c>
       <c r="C5" s="1">
-        <v>-20.3</v>
+        <v>-20</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="10">
@@ -4937,7 +4937,7 @@
       </c>
       <c r="L5">
         <f xml:space="preserve"> F5 - ABS(C5)</f>
-        <v>3.5749999999999993</v>
+        <v>3.875</v>
       </c>
       <c r="M5">
         <f t="shared" si="1"/>
@@ -5042,7 +5042,7 @@
       <c r="F12" s="1"/>
       <c r="L12">
         <f>L8-L20</f>
-        <v>-0.8000000000000016</v>
+        <v>-0.90000000000000036</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -5093,7 +5093,7 @@
         <v>47.625</v>
       </c>
       <c r="K15">
-        <f t="shared" ref="K15" si="6" xml:space="preserve"> E15 - ABS(B15)</f>
+        <f xml:space="preserve"> E15 - ABS(B15)</f>
         <v>0.42499999999999716</v>
       </c>
       <c r="L15">
@@ -5101,7 +5101,7 @@
         <v>-0.17499999999999716</v>
       </c>
       <c r="M15">
-        <f t="shared" ref="M15" si="7" xml:space="preserve"> G15 - ABS(D15)</f>
+        <f t="shared" ref="M15" si="6" xml:space="preserve"> G15 - ABS(D15)</f>
         <v>0</v>
       </c>
     </row>
@@ -5116,59 +5116,59 @@
     <row r="20" spans="1:16">
       <c r="K20">
         <f>AVERAGE(K2:K5)</f>
-        <v>-8.1249999999999822E-2</v>
+        <v>4.3749999999999289E-2</v>
       </c>
       <c r="L20">
         <f>AVERAGE(L2:L5)</f>
-        <v>3.5750000000000002</v>
+        <v>3.6749999999999989</v>
       </c>
       <c r="O20">
         <f>K46-K20</f>
-        <v>-0.19375000000000053</v>
+        <v>-0.31874999999999964</v>
       </c>
       <c r="P20">
         <f>L20-L46</f>
-        <v>0.4250000000000016</v>
+        <v>0.52500000000000036</v>
       </c>
     </row>
     <row r="22" spans="1:16">
       <c r="K22">
         <f>K30-$K$20</f>
-        <v>0.65624999999999911</v>
+        <v>0.53125</v>
       </c>
       <c r="L22">
         <f>L2-$L$20</f>
-        <v>4.9999999999999822E-2</v>
+        <v>-4.9999999999998934E-2</v>
       </c>
     </row>
     <row r="23" spans="1:16">
       <c r="K23">
         <f>K31-$K$20</f>
-        <v>0.20624999999999982</v>
+        <v>8.1250000000000711E-2</v>
       </c>
       <c r="L23">
         <f>L3-$L$20</f>
-        <v>-0.45000000000000018</v>
+        <v>-0.25000000000000178</v>
       </c>
     </row>
     <row r="24" spans="1:16">
       <c r="K24">
         <f>K32-$K$20</f>
-        <v>-0.74374999999999947</v>
+        <v>-0.86874999999999858</v>
       </c>
       <c r="L24">
         <f>L4-$L$20</f>
-        <v>0.40000000000000124</v>
+        <v>9.9999999999999645E-2</v>
       </c>
     </row>
     <row r="25" spans="1:16">
       <c r="K25">
         <f>K33-$K$20</f>
-        <v>-0.8937500000000016</v>
+        <v>-1.0187500000000007</v>
       </c>
       <c r="L25">
         <f>L5-$L$20</f>
-        <v>0</v>
+        <v>0.20000000000000107</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -5203,7 +5203,7 @@
         <v>3.4249999999999972</v>
       </c>
       <c r="M30">
-        <f t="shared" ref="M30:M33" si="8" xml:space="preserve"> G30 - ABS(D30)</f>
+        <f t="shared" ref="M30:M33" si="7" xml:space="preserve"> G30 - ABS(D30)</f>
         <v>0</v>
       </c>
     </row>
@@ -5225,7 +5225,7 @@
         <v>47.625</v>
       </c>
       <c r="K31">
-        <f t="shared" ref="K31" si="9" xml:space="preserve"> E31 - ABS(B31)</f>
+        <f t="shared" ref="K31" si="8" xml:space="preserve"> E31 - ABS(B31)</f>
         <v>0.125</v>
       </c>
       <c r="L31">
@@ -5233,7 +5233,7 @@
         <v>3.0249999999999986</v>
       </c>
       <c r="M31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -5259,11 +5259,11 @@
         <v>-0.82499999999999929</v>
       </c>
       <c r="L32">
-        <f t="shared" ref="L32" si="10" xml:space="preserve"> F32 - ABS(C32)</f>
+        <f t="shared" ref="L32" si="9" xml:space="preserve"> F32 - ABS(C32)</f>
         <v>3.5749999999999993</v>
       </c>
       <c r="M32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -5293,7 +5293,7 @@
         <v>2.5749999999999993</v>
       </c>
       <c r="M33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -5326,15 +5326,15 @@
         <v>40.5</v>
       </c>
       <c r="K36">
-        <f t="shared" ref="K36" si="11" xml:space="preserve"> E36 - ABS(B36)</f>
+        <f t="shared" ref="K36" si="10" xml:space="preserve"> E36 - ABS(B36)</f>
         <v>0.60000000000000142</v>
       </c>
       <c r="L36">
-        <f t="shared" ref="L36" si="12" xml:space="preserve"> F36 - ABS(C36)</f>
+        <f t="shared" ref="L36" si="11" xml:space="preserve"> F36 - ABS(C36)</f>
         <v>-9.1000000000000014</v>
       </c>
       <c r="M36">
-        <f t="shared" ref="M36" si="13" xml:space="preserve"> G36 - ABS(D36)</f>
+        <f t="shared" ref="M36" si="12" xml:space="preserve"> G36 - ABS(D36)</f>
         <v>0</v>
       </c>
     </row>
@@ -5346,11 +5346,11 @@
     <row r="39" spans="1:13">
       <c r="K39">
         <f>K36-K20</f>
-        <v>0.68125000000000124</v>
+        <v>0.55625000000000213</v>
       </c>
       <c r="L39">
         <f>L36-L20</f>
-        <v>-12.675000000000001</v>
+        <v>-12.775</v>
       </c>
     </row>
     <row r="45" spans="1:13">
@@ -5374,7 +5374,7 @@
     <row r="48" spans="1:13">
       <c r="K48">
         <f>K30-$K$20</f>
-        <v>0.65624999999999911</v>
+        <v>0.53125</v>
       </c>
       <c r="L48">
         <f>L30-$L$46</f>
@@ -5383,31 +5383,31 @@
     </row>
     <row r="49" spans="11:12">
       <c r="K49">
-        <f t="shared" ref="K49:K51" si="14">K31-$K$20</f>
-        <v>0.20624999999999982</v>
+        <f t="shared" ref="K49:K51" si="13">K31-$K$20</f>
+        <v>8.1250000000000711E-2</v>
       </c>
       <c r="L49">
-        <f t="shared" ref="L49:L51" si="15">L31-$L$46</f>
+        <f t="shared" ref="L49:L51" si="14">L31-$L$46</f>
         <v>-0.125</v>
       </c>
     </row>
     <row r="50" spans="11:12">
       <c r="K50">
+        <f t="shared" si="13"/>
+        <v>-0.86874999999999858</v>
+      </c>
+      <c r="L50">
         <f t="shared" si="14"/>
-        <v>-0.74374999999999947</v>
-      </c>
-      <c r="L50">
-        <f t="shared" si="15"/>
         <v>0.42500000000000071</v>
       </c>
     </row>
     <row r="51" spans="11:12">
       <c r="K51">
+        <f t="shared" si="13"/>
+        <v>-1.0187500000000007</v>
+      </c>
+      <c r="L51">
         <f t="shared" si="14"/>
-        <v>-0.8937500000000016</v>
-      </c>
-      <c r="L51">
-        <f t="shared" si="15"/>
         <v>-0.57499999999999929</v>
       </c>
     </row>
@@ -5419,40 +5419,40 @@
     <row r="55" spans="11:12">
       <c r="K55">
         <f>K30-$K$20</f>
-        <v>0.65624999999999911</v>
+        <v>0.53125</v>
       </c>
       <c r="L55">
         <f>L30-$L$20</f>
-        <v>-0.15000000000000302</v>
+        <v>-0.25000000000000178</v>
       </c>
     </row>
     <row r="56" spans="11:12">
       <c r="K56">
-        <f t="shared" ref="K56:K57" si="16">K31-$K$20</f>
-        <v>0.20624999999999982</v>
+        <f t="shared" ref="K56:K57" si="15">K31-$K$20</f>
+        <v>8.1250000000000711E-2</v>
       </c>
       <c r="L56">
-        <f t="shared" ref="L56:L58" si="17">L38-$L$46</f>
+        <f t="shared" ref="L56:L58" si="16">L38-$L$46</f>
         <v>-3.1499999999999986</v>
       </c>
     </row>
     <row r="57" spans="11:12">
       <c r="K57">
+        <f t="shared" si="15"/>
+        <v>-0.86874999999999858</v>
+      </c>
+      <c r="L57">
         <f t="shared" si="16"/>
-        <v>-0.74374999999999947</v>
-      </c>
-      <c r="L57">
-        <f t="shared" si="17"/>
-        <v>-15.824999999999999</v>
+        <v>-15.924999999999999</v>
       </c>
     </row>
     <row r="58" spans="11:12">
       <c r="K58">
         <f>K33-$K$20</f>
-        <v>-0.8937500000000016</v>
+        <v>-1.0187500000000007</v>
       </c>
       <c r="L58">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>-3.1499999999999986</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adds function to calculate the deltas for our four given points
</commit_message>
<xml_diff>
--- a/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
+++ b/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/Dropbox/Brain Stormz FTC/2023-24-code/AprilTag Performance Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC98E399-4F9F-914F-A279-F0D0F5DE234E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCCA7E4-30A9-2B41-BB0D-AAABA60F5D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="3940" windowWidth="28800" windowHeight="14660" activeTab="7" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="14660" activeTab="7" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="118">
   <si>
     <t>Point</t>
   </si>
@@ -382,9 +382,6 @@
     <t>AVG X ERR</t>
   </si>
   <si>
-    <t>PROCESSED</t>
-  </si>
-  <si>
     <t>SPIKE (B5) - important point</t>
   </si>
   <si>
@@ -398,9 +395,6 @@
   </si>
   <si>
     <t>R4</t>
-  </si>
-  <si>
-    <t>BLAH1</t>
   </si>
   <si>
     <t>BUT WITH THE FIRST</t>
@@ -4788,8 +4782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2014BCED-35E7-FE44-9FDA-065FB736E196}">
   <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="83" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4825,10 +4819,10 @@
         <v>107</v>
       </c>
       <c r="B2" s="1">
-        <v>48</v>
+        <v>47.7</v>
       </c>
       <c r="C2" s="1">
-        <v>-44</v>
+        <v>-47.8</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="10">
@@ -4839,11 +4833,11 @@
       </c>
       <c r="K2">
         <f xml:space="preserve"> E2 - ABS(B2)</f>
-        <v>-0.5</v>
+        <v>-0.20000000000000284</v>
       </c>
       <c r="L2">
         <f xml:space="preserve"> F2 - ABS(C2)</f>
-        <v>3.625</v>
+        <v>-0.17499999999999716</v>
       </c>
       <c r="M2">
         <f t="shared" ref="M2" si="0" xml:space="preserve"> G2 - ABS(D2)</f>
@@ -4855,7 +4849,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="1">
-        <v>23.5</v>
+        <v>23.4</v>
       </c>
       <c r="C3" s="1">
         <v>-44.2</v>
@@ -4873,7 +4867,7 @@
       </c>
       <c r="K3">
         <f xml:space="preserve"> E3 - ABS(B3)</f>
-        <v>0.125</v>
+        <v>0.22500000000000142</v>
       </c>
       <c r="L3">
         <f xml:space="preserve"> F3 - ABS(C3)</f>
@@ -4985,7 +4979,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B8" s="1">
         <v>14.4</v>
@@ -5042,7 +5036,7 @@
       <c r="F12" s="1"/>
       <c r="L12">
         <f>L8-L20</f>
-        <v>-0.90000000000000036</v>
+        <v>4.9999999999998934E-2</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -5077,7 +5071,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B15" s="1">
         <v>-47.2</v>
@@ -5116,59 +5110,59 @@
     <row r="20" spans="1:16">
       <c r="K20">
         <f>AVERAGE(K2:K5)</f>
-        <v>4.3749999999999289E-2</v>
+        <v>0.14374999999999893</v>
       </c>
       <c r="L20">
         <f>AVERAGE(L2:L5)</f>
-        <v>3.6749999999999989</v>
+        <v>2.7249999999999996</v>
       </c>
       <c r="O20">
         <f>K46-K20</f>
-        <v>-0.31874999999999964</v>
+        <v>-0.39374999999999893</v>
       </c>
       <c r="P20">
         <f>L20-L46</f>
-        <v>0.52500000000000036</v>
+        <v>-0.59999999999999876</v>
       </c>
     </row>
     <row r="22" spans="1:16">
       <c r="K22">
         <f>K30-$K$20</f>
-        <v>0.53125</v>
+        <v>0.13124999999999964</v>
       </c>
       <c r="L22">
         <f>L2-$L$20</f>
-        <v>-4.9999999999998934E-2</v>
+        <v>-2.8999999999999968</v>
       </c>
     </row>
     <row r="23" spans="1:16">
       <c r="K23">
         <f>K31-$K$20</f>
-        <v>8.1250000000000711E-2</v>
+        <v>-0.21875000000000178</v>
       </c>
       <c r="L23">
         <f>L3-$L$20</f>
-        <v>-0.25000000000000178</v>
+        <v>0.69999999999999751</v>
       </c>
     </row>
     <row r="24" spans="1:16">
       <c r="K24">
         <f>K32-$K$20</f>
-        <v>-0.86874999999999858</v>
+        <v>-0.66874999999999751</v>
       </c>
       <c r="L24">
         <f>L4-$L$20</f>
-        <v>9.9999999999999645E-2</v>
+        <v>1.0499999999999989</v>
       </c>
     </row>
     <row r="25" spans="1:16">
       <c r="K25">
         <f>K33-$K$20</f>
-        <v>-1.0187500000000007</v>
+        <v>-0.81874999999999609</v>
       </c>
       <c r="L25">
         <f>L5-$L$20</f>
-        <v>0.20000000000000107</v>
+        <v>1.1500000000000004</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -5179,28 +5173,28 @@
     </row>
     <row r="30" spans="1:16">
       <c r="A30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B30" s="1">
-        <v>-23.3</v>
+        <v>-23.6</v>
       </c>
       <c r="C30" s="1">
-        <v>-44.2</v>
+        <v>-44.1</v>
       </c>
       <c r="D30" s="1"/>
-      <c r="E30" s="11">
+      <c r="E30" s="10">
         <v>23.875</v>
       </c>
-      <c r="F30" s="11">
+      <c r="F30" s="10">
         <v>47.625</v>
       </c>
       <c r="K30">
         <f xml:space="preserve"> E30 - ABS(B30)</f>
-        <v>0.57499999999999929</v>
+        <v>0.27499999999999858</v>
       </c>
       <c r="L30">
         <f xml:space="preserve"> F30 - ABS(C30)</f>
-        <v>3.4249999999999972</v>
+        <v>3.5249999999999986</v>
       </c>
       <c r="M30">
         <f t="shared" ref="M30:M33" si="7" xml:space="preserve"> G30 - ABS(D30)</f>
@@ -5209,28 +5203,28 @@
     </row>
     <row r="31" spans="1:16">
       <c r="A31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B31" s="1">
-        <v>-47.5</v>
+        <v>-47.7</v>
       </c>
       <c r="C31" s="1">
-        <v>-44.6</v>
+        <v>-44.7</v>
       </c>
       <c r="D31" s="1"/>
-      <c r="E31" s="11">
+      <c r="E31" s="10">
         <v>47.625</v>
       </c>
-      <c r="F31" s="11">
+      <c r="F31" s="10">
         <v>47.625</v>
       </c>
       <c r="K31">
-        <f t="shared" ref="K31" si="8" xml:space="preserve"> E31 - ABS(B31)</f>
-        <v>0.125</v>
+        <f xml:space="preserve"> E31 - ABS(B31)</f>
+        <v>-7.5000000000002842E-2</v>
       </c>
       <c r="L31">
         <f xml:space="preserve"> F31 - ABS(C31)</f>
-        <v>3.0249999999999986</v>
+        <v>2.9249999999999972</v>
       </c>
       <c r="M31">
         <f t="shared" si="7"/>
@@ -5239,27 +5233,27 @@
     </row>
     <row r="32" spans="1:16">
       <c r="A32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B32" s="1">
-        <v>-24.7</v>
+        <v>-24.4</v>
       </c>
       <c r="C32" s="1">
         <v>-19.8</v>
       </c>
       <c r="D32" s="1"/>
-      <c r="E32" s="11">
+      <c r="E32" s="10">
         <v>23.875</v>
       </c>
-      <c r="F32" s="11">
+      <c r="F32" s="10">
         <v>23.375</v>
       </c>
       <c r="K32">
         <f xml:space="preserve"> E32 - ABS(B32)</f>
-        <v>-0.82499999999999929</v>
+        <v>-0.52499999999999858</v>
       </c>
       <c r="L32">
-        <f t="shared" ref="L32" si="9" xml:space="preserve"> F32 - ABS(C32)</f>
+        <f xml:space="preserve"> F32 - ABS(C32)</f>
         <v>3.5749999999999993</v>
       </c>
       <c r="M32">
@@ -5269,28 +5263,28 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B33" s="1">
-        <v>-48.6</v>
+        <v>-48.3</v>
       </c>
       <c r="C33" s="1">
-        <v>-20.8</v>
+        <v>-20.100000000000001</v>
       </c>
       <c r="D33" s="1"/>
-      <c r="E33" s="11">
+      <c r="E33" s="10">
         <v>47.625</v>
       </c>
-      <c r="F33" s="11">
+      <c r="F33" s="10">
         <v>23.375</v>
       </c>
       <c r="K33">
         <f xml:space="preserve"> E33 - ABS(B33)</f>
-        <v>-0.97500000000000142</v>
+        <v>-0.67499999999999716</v>
       </c>
       <c r="L33">
         <f xml:space="preserve"> F33 - ABS(C33)</f>
-        <v>2.5749999999999993</v>
+        <v>3.2749999999999986</v>
       </c>
       <c r="M33">
         <f t="shared" si="7"/>
@@ -5310,48 +5304,10 @@
       <c r="J34" s="8"/>
     </row>
     <row r="36" spans="1:13">
-      <c r="A36" t="s">
-        <v>118</v>
-      </c>
-      <c r="B36" s="1">
-        <v>-34.4</v>
-      </c>
-      <c r="C36" s="1">
-        <v>-49.6</v>
-      </c>
-      <c r="E36" s="11">
-        <v>35</v>
-      </c>
-      <c r="F36" s="11">
-        <v>40.5</v>
-      </c>
-      <c r="K36">
-        <f t="shared" ref="K36" si="10" xml:space="preserve"> E36 - ABS(B36)</f>
-        <v>0.60000000000000142</v>
-      </c>
-      <c r="L36">
-        <f t="shared" ref="L36" si="11" xml:space="preserve"> F36 - ABS(C36)</f>
-        <v>-9.1000000000000014</v>
-      </c>
-      <c r="M36">
-        <f t="shared" ref="M36" si="12" xml:space="preserve"> G36 - ABS(D36)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="K37" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="K39">
-        <f>K36-K20</f>
-        <v>0.55625000000000213</v>
-      </c>
-      <c r="L39">
-        <f>L36-L20</f>
-        <v>-12.775</v>
-      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
     </row>
     <row r="45" spans="1:13">
       <c r="K45" t="s">
@@ -5364,96 +5320,96 @@
     <row r="46" spans="1:13">
       <c r="K46">
         <f>AVERAGE(K30:K33)</f>
-        <v>-0.27500000000000036</v>
+        <v>-0.25</v>
       </c>
       <c r="L46">
         <f>AVERAGE(L30:L33)</f>
-        <v>3.1499999999999986</v>
+        <v>3.3249999999999984</v>
       </c>
     </row>
     <row r="48" spans="1:13">
       <c r="K48">
         <f>K30-$K$20</f>
-        <v>0.53125</v>
+        <v>0.13124999999999964</v>
       </c>
       <c r="L48">
         <f>L30-$L$46</f>
-        <v>0.27499999999999858</v>
+        <v>0.20000000000000018</v>
       </c>
     </row>
     <row r="49" spans="11:12">
       <c r="K49">
-        <f t="shared" ref="K49:K51" si="13">K31-$K$20</f>
-        <v>8.1250000000000711E-2</v>
+        <f t="shared" ref="K49:K51" si="8">K31-$K$20</f>
+        <v>-0.21875000000000178</v>
       </c>
       <c r="L49">
-        <f t="shared" ref="L49:L51" si="14">L31-$L$46</f>
-        <v>-0.125</v>
+        <f t="shared" ref="L49:L51" si="9">L31-$L$46</f>
+        <v>-0.40000000000000124</v>
       </c>
     </row>
     <row r="50" spans="11:12">
       <c r="K50">
-        <f t="shared" si="13"/>
-        <v>-0.86874999999999858</v>
+        <f t="shared" si="8"/>
+        <v>-0.66874999999999751</v>
       </c>
       <c r="L50">
-        <f t="shared" si="14"/>
-        <v>0.42500000000000071</v>
+        <f t="shared" si="9"/>
+        <v>0.25000000000000089</v>
       </c>
     </row>
     <row r="51" spans="11:12">
       <c r="K51">
-        <f t="shared" si="13"/>
-        <v>-1.0187500000000007</v>
+        <f t="shared" si="8"/>
+        <v>-0.81874999999999609</v>
       </c>
       <c r="L51">
-        <f t="shared" si="14"/>
-        <v>-0.57499999999999929</v>
+        <f t="shared" si="9"/>
+        <v>-4.9999999999999822E-2</v>
       </c>
     </row>
     <row r="53" spans="11:12">
       <c r="K53" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="11:12">
       <c r="K55">
         <f>K30-$K$20</f>
-        <v>0.53125</v>
+        <v>0.13124999999999964</v>
       </c>
       <c r="L55">
         <f>L30-$L$20</f>
-        <v>-0.25000000000000178</v>
+        <v>0.79999999999999893</v>
       </c>
     </row>
     <row r="56" spans="11:12">
       <c r="K56">
-        <f t="shared" ref="K56:K57" si="15">K31-$K$20</f>
-        <v>8.1250000000000711E-2</v>
+        <f t="shared" ref="K56:K57" si="10">K31-$K$20</f>
+        <v>-0.21875000000000178</v>
       </c>
       <c r="L56">
-        <f t="shared" ref="L56:L58" si="16">L38-$L$46</f>
-        <v>-3.1499999999999986</v>
+        <f t="shared" ref="L56:L58" si="11">L38-$L$46</f>
+        <v>-3.3249999999999984</v>
       </c>
     </row>
     <row r="57" spans="11:12">
       <c r="K57">
-        <f t="shared" si="15"/>
-        <v>-0.86874999999999858</v>
+        <f t="shared" si="10"/>
+        <v>-0.66874999999999751</v>
       </c>
       <c r="L57">
-        <f t="shared" si="16"/>
-        <v>-15.924999999999999</v>
+        <f t="shared" si="11"/>
+        <v>-3.3249999999999984</v>
       </c>
     </row>
     <row r="58" spans="11:12">
       <c r="K58">
         <f>K33-$K$20</f>
-        <v>-1.0187500000000007</v>
+        <v>-0.81874999999999609</v>
       </c>
       <c r="L58">
-        <f t="shared" si="16"/>
-        <v>-3.1499999999999986</v>
+        <f t="shared" si="11"/>
+        <v>-3.3249999999999984</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fully working Calibration - Four Buttons + Annotations (slate) Version
</commit_message>
<xml_diff>
--- a/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
+++ b/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/Dropbox/Brain Stormz FTC/2023-24-code/AprilTag Performance Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCCA7E4-30A9-2B41-BB0D-AAABA60F5D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74911A83-DBBF-2249-A81A-6CBF8EBB834F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="14660" activeTab="7" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
+    <workbookView xWindow="8860" yWindow="500" windowWidth="19940" windowHeight="14660" activeTab="7" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4782,8 +4782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2014BCED-35E7-FE44-9FDA-065FB736E196}">
   <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="83" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4819,10 +4819,10 @@
         <v>107</v>
       </c>
       <c r="B2" s="1">
-        <v>47.7</v>
+        <v>-49.3</v>
       </c>
       <c r="C2" s="1">
-        <v>-47.8</v>
+        <v>-47.7</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="10">
@@ -4833,11 +4833,11 @@
       </c>
       <c r="K2">
         <f xml:space="preserve"> E2 - ABS(B2)</f>
-        <v>-0.20000000000000284</v>
+        <v>-1.7999999999999972</v>
       </c>
       <c r="L2">
         <f xml:space="preserve"> F2 - ABS(C2)</f>
-        <v>-0.17499999999999716</v>
+        <v>-7.5000000000002842E-2</v>
       </c>
       <c r="M2">
         <f t="shared" ref="M2" si="0" xml:space="preserve"> G2 - ABS(D2)</f>
@@ -4849,10 +4849,10 @@
         <v>28</v>
       </c>
       <c r="B3" s="1">
-        <v>23.4</v>
+        <v>23.5</v>
       </c>
       <c r="C3" s="1">
-        <v>-44.2</v>
+        <v>-48.2</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="10">
@@ -4867,11 +4867,11 @@
       </c>
       <c r="K3">
         <f xml:space="preserve"> E3 - ABS(B3)</f>
-        <v>0.22500000000000142</v>
+        <v>0.125</v>
       </c>
       <c r="L3">
         <f xml:space="preserve"> F3 - ABS(C3)</f>
-        <v>3.4249999999999972</v>
+        <v>-0.57500000000000284</v>
       </c>
       <c r="M3">
         <f t="shared" ref="M3:M6" si="1" xml:space="preserve"> G3 - ABS(D3)</f>
@@ -4883,10 +4883,10 @@
         <v>108</v>
       </c>
       <c r="B4" s="1">
-        <v>47.1</v>
+        <v>47.9</v>
       </c>
       <c r="C4" s="1">
-        <v>-20.100000000000001</v>
+        <v>-23.6</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="10">
@@ -4897,11 +4897,11 @@
       </c>
       <c r="K4">
         <f xml:space="preserve"> E4 - ABS(B4)</f>
-        <v>0.39999999999999858</v>
+        <v>-0.39999999999999858</v>
       </c>
       <c r="L4">
         <f xml:space="preserve"> F4 - ABS(C4)</f>
-        <v>3.7749999999999986</v>
+        <v>0.27499999999999858</v>
       </c>
       <c r="M4">
         <f t="shared" si="1"/>
@@ -4916,7 +4916,7 @@
         <v>23.6</v>
       </c>
       <c r="C5" s="1">
-        <v>-20</v>
+        <v>-23.3</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="10">
@@ -4931,7 +4931,7 @@
       </c>
       <c r="L5">
         <f xml:space="preserve"> F5 - ABS(C5)</f>
-        <v>3.875</v>
+        <v>0.57499999999999929</v>
       </c>
       <c r="M5">
         <f t="shared" si="1"/>
@@ -5036,7 +5036,7 @@
       <c r="F12" s="1"/>
       <c r="L12">
         <f>L8-L20</f>
-        <v>4.9999999999998934E-2</v>
+        <v>2.7250000000000005</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -5110,59 +5110,59 @@
     <row r="20" spans="1:16">
       <c r="K20">
         <f>AVERAGE(K2:K5)</f>
-        <v>0.14374999999999893</v>
+        <v>-0.48124999999999929</v>
       </c>
       <c r="L20">
         <f>AVERAGE(L2:L5)</f>
-        <v>2.7249999999999996</v>
+        <v>4.9999999999998046E-2</v>
       </c>
       <c r="O20">
         <f>K46-K20</f>
-        <v>-0.39374999999999893</v>
+        <v>0.90624999999999822</v>
       </c>
       <c r="P20">
         <f>L20-L46</f>
-        <v>-0.59999999999999876</v>
+        <v>-0.15000000000000213</v>
       </c>
     </row>
     <row r="22" spans="1:16">
       <c r="K22">
         <f>K30-$K$20</f>
-        <v>0.13124999999999964</v>
+        <v>1.3562499999999993</v>
       </c>
       <c r="L22">
         <f>L2-$L$20</f>
-        <v>-2.8999999999999968</v>
+        <v>-0.12500000000000089</v>
       </c>
     </row>
     <row r="23" spans="1:16">
       <c r="K23">
         <f>K31-$K$20</f>
-        <v>-0.21875000000000178</v>
+        <v>1.0062499999999979</v>
       </c>
       <c r="L23">
         <f>L3-$L$20</f>
-        <v>0.69999999999999751</v>
+        <v>-0.62500000000000089</v>
       </c>
     </row>
     <row r="24" spans="1:16">
       <c r="K24">
         <f>K32-$K$20</f>
-        <v>-0.66874999999999751</v>
+        <v>-0.14375000000000071</v>
       </c>
       <c r="L24">
         <f>L4-$L$20</f>
-        <v>1.0499999999999989</v>
+        <v>0.22500000000000053</v>
       </c>
     </row>
     <row r="25" spans="1:16">
       <c r="K25">
         <f>K33-$K$20</f>
-        <v>-0.81874999999999609</v>
+        <v>1.4062499999999964</v>
       </c>
       <c r="L25">
         <f>L5-$L$20</f>
-        <v>1.1500000000000004</v>
+        <v>0.52500000000000124</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -5176,10 +5176,10 @@
         <v>113</v>
       </c>
       <c r="B30" s="1">
-        <v>-23.6</v>
+        <v>-23</v>
       </c>
       <c r="C30" s="1">
-        <v>-44.1</v>
+        <v>-47.4</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="10">
@@ -5190,11 +5190,11 @@
       </c>
       <c r="K30">
         <f xml:space="preserve"> E30 - ABS(B30)</f>
-        <v>0.27499999999999858</v>
+        <v>0.875</v>
       </c>
       <c r="L30">
         <f xml:space="preserve"> F30 - ABS(C30)</f>
-        <v>3.5249999999999986</v>
+        <v>0.22500000000000142</v>
       </c>
       <c r="M30">
         <f t="shared" ref="M30:M33" si="7" xml:space="preserve"> G30 - ABS(D30)</f>
@@ -5206,10 +5206,10 @@
         <v>114</v>
       </c>
       <c r="B31" s="1">
-        <v>-47.7</v>
+        <v>-47.1</v>
       </c>
       <c r="C31" s="1">
-        <v>-44.7</v>
+        <v>-47.6</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="10">
@@ -5220,11 +5220,11 @@
       </c>
       <c r="K31">
         <f xml:space="preserve"> E31 - ABS(B31)</f>
-        <v>-7.5000000000002842E-2</v>
+        <v>0.52499999999999858</v>
       </c>
       <c r="L31">
         <f xml:space="preserve"> F31 - ABS(C31)</f>
-        <v>2.9249999999999972</v>
+        <v>2.4999999999998579E-2</v>
       </c>
       <c r="M31">
         <f t="shared" si="7"/>
@@ -5236,10 +5236,10 @@
         <v>115</v>
       </c>
       <c r="B32" s="1">
-        <v>-24.4</v>
+        <v>-24.5</v>
       </c>
       <c r="C32" s="1">
-        <v>-19.8</v>
+        <v>-23</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="10">
@@ -5250,11 +5250,11 @@
       </c>
       <c r="K32">
         <f xml:space="preserve"> E32 - ABS(B32)</f>
-        <v>-0.52499999999999858</v>
+        <v>-0.625</v>
       </c>
       <c r="L32">
         <f xml:space="preserve"> F32 - ABS(C32)</f>
-        <v>3.5749999999999993</v>
+        <v>0.375</v>
       </c>
       <c r="M32">
         <f t="shared" si="7"/>
@@ -5266,10 +5266,10 @@
         <v>116</v>
       </c>
       <c r="B33" s="1">
-        <v>-48.3</v>
+        <v>-46.7</v>
       </c>
       <c r="C33" s="1">
-        <v>-20.100000000000001</v>
+        <v>-23.2</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="10">
@@ -5280,11 +5280,11 @@
       </c>
       <c r="K33">
         <f xml:space="preserve"> E33 - ABS(B33)</f>
-        <v>-0.67499999999999716</v>
+        <v>0.92499999999999716</v>
       </c>
       <c r="L33">
         <f xml:space="preserve"> F33 - ABS(C33)</f>
-        <v>3.2749999999999986</v>
+        <v>0.17500000000000071</v>
       </c>
       <c r="M33">
         <f t="shared" si="7"/>
@@ -5320,51 +5320,51 @@
     <row r="46" spans="1:13">
       <c r="K46">
         <f>AVERAGE(K30:K33)</f>
-        <v>-0.25</v>
+        <v>0.42499999999999893</v>
       </c>
       <c r="L46">
         <f>AVERAGE(L30:L33)</f>
-        <v>3.3249999999999984</v>
+        <v>0.20000000000000018</v>
       </c>
     </row>
     <row r="48" spans="1:13">
       <c r="K48">
         <f>K30-$K$20</f>
-        <v>0.13124999999999964</v>
+        <v>1.3562499999999993</v>
       </c>
       <c r="L48">
         <f>L30-$L$46</f>
-        <v>0.20000000000000018</v>
+        <v>2.5000000000001243E-2</v>
       </c>
     </row>
     <row r="49" spans="11:12">
       <c r="K49">
         <f t="shared" ref="K49:K51" si="8">K31-$K$20</f>
-        <v>-0.21875000000000178</v>
+        <v>1.0062499999999979</v>
       </c>
       <c r="L49">
         <f t="shared" ref="L49:L51" si="9">L31-$L$46</f>
-        <v>-0.40000000000000124</v>
+        <v>-0.1750000000000016</v>
       </c>
     </row>
     <row r="50" spans="11:12">
       <c r="K50">
         <f t="shared" si="8"/>
-        <v>-0.66874999999999751</v>
+        <v>-0.14375000000000071</v>
       </c>
       <c r="L50">
         <f t="shared" si="9"/>
-        <v>0.25000000000000089</v>
+        <v>0.17499999999999982</v>
       </c>
     </row>
     <row r="51" spans="11:12">
       <c r="K51">
         <f t="shared" si="8"/>
-        <v>-0.81874999999999609</v>
+        <v>1.4062499999999964</v>
       </c>
       <c r="L51">
         <f t="shared" si="9"/>
-        <v>-4.9999999999999822E-2</v>
+        <v>-2.4999999999999467E-2</v>
       </c>
     </row>
     <row r="53" spans="11:12">
@@ -5375,41 +5375,41 @@
     <row r="55" spans="11:12">
       <c r="K55">
         <f>K30-$K$20</f>
-        <v>0.13124999999999964</v>
+        <v>1.3562499999999993</v>
       </c>
       <c r="L55">
         <f>L30-$L$20</f>
-        <v>0.79999999999999893</v>
+        <v>0.17500000000000338</v>
       </c>
     </row>
     <row r="56" spans="11:12">
       <c r="K56">
         <f t="shared" ref="K56:K57" si="10">K31-$K$20</f>
-        <v>-0.21875000000000178</v>
+        <v>1.0062499999999979</v>
       </c>
       <c r="L56">
         <f t="shared" ref="L56:L58" si="11">L38-$L$46</f>
-        <v>-3.3249999999999984</v>
+        <v>-0.20000000000000018</v>
       </c>
     </row>
     <row r="57" spans="11:12">
       <c r="K57">
         <f t="shared" si="10"/>
-        <v>-0.66874999999999751</v>
+        <v>-0.14375000000000071</v>
       </c>
       <c r="L57">
         <f t="shared" si="11"/>
-        <v>-3.3249999999999984</v>
+        <v>-0.20000000000000018</v>
       </c>
     </row>
     <row r="58" spans="11:12">
       <c r="K58">
         <f>K33-$K$20</f>
-        <v>-0.81874999999999609</v>
+        <v>1.4062499999999964</v>
       </c>
       <c r="L58">
         <f t="shared" si="11"/>
-        <v>-3.3249999999999984</v>
+        <v>-0.20000000000000018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
calibration system still broken, but now we have a good calibration
</commit_message>
<xml_diff>
--- a/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
+++ b/AprilTag Performance Evaluation/30-3-24 AprilTag With Best Tag Finder.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/Dropbox/Brain Stormz FTC/2023-24-code/AprilTag Performance Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0CEB81-9710-874C-91C0-FB36EAF92D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D45E4EC-6D4B-B946-B4AB-33094734F610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8860" yWindow="500" windowWidth="19940" windowHeight="16280" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
+    <workbookView xWindow="-40" yWindow="500" windowWidth="19940" windowHeight="16280" xr2:uid="{0242ED38-B07D-D24A-BFD7-C5D111369A13}"/>
   </bookViews>
   <sheets>
     <sheet name="Worlds-like test" sheetId="8" r:id="rId1"/>
+    <sheet name="Sheet9" sheetId="10" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Real Y</t>
   </si>
@@ -109,7 +110,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -124,6 +125,12 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF2AACB8"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFFFF00"/>
       <name val="Menlo"/>
@@ -134,6 +141,12 @@
       <color theme="1"/>
       <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFBCBEC4"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -162,14 +175,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,17 +521,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2014BCED-35E7-FE44-9FDA-065FB736E196}">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="11" max="11" width="12.5" customWidth="1"/>
     <col min="12" max="12" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -542,51 +557,51 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1">
-        <v>47.68</v>
+        <v>47.9</v>
       </c>
       <c r="C2" s="1">
-        <v>-44.56</v>
+        <v>-47.6</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>47.5</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="3">
         <v>47.625</v>
       </c>
       <c r="K2">
         <f xml:space="preserve"> E2 - ABS(B2)</f>
-        <v>-0.17999999999999972</v>
+        <v>-0.39999999999999858</v>
       </c>
       <c r="L2">
         <f xml:space="preserve"> F2 - ABS(C2)</f>
-        <v>3.0649999999999977</v>
+        <v>2.4999999999998579E-2</v>
       </c>
       <c r="M2">
         <f t="shared" ref="M2" si="0" xml:space="preserve"> G2 - ABS(D2)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>23.66</v>
+        <v>23.4</v>
       </c>
       <c r="C3" s="1">
-        <v>-44.53</v>
+        <v>-47.9</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>23.625</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="3">
         <v>47.625</v>
       </c>
       <c r="H3">
@@ -595,108 +610,108 @@
       </c>
       <c r="K3">
         <f xml:space="preserve"> E3 - ABS(B3)</f>
-        <v>-3.5000000000000142E-2</v>
+        <v>0.22500000000000142</v>
       </c>
       <c r="L3">
         <f xml:space="preserve"> F3 - ABS(C3)</f>
-        <v>3.0949999999999989</v>
+        <v>-0.27499999999999858</v>
       </c>
       <c r="M3">
         <f t="shared" ref="M3:M5" si="1" xml:space="preserve"> G3 - ABS(D3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1">
-        <v>48.69</v>
+        <v>48.1</v>
       </c>
       <c r="C4" s="1">
-        <v>-20.55</v>
+        <v>-23.2</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>47.5</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="3">
         <v>23.875</v>
       </c>
       <c r="K4">
         <f xml:space="preserve"> E4 - ABS(B4)</f>
-        <v>-1.1899999999999977</v>
+        <v>-0.60000000000000142</v>
       </c>
       <c r="L4">
         <f xml:space="preserve"> F4 - ABS(C4)</f>
-        <v>3.3249999999999993</v>
+        <v>0.67500000000000071</v>
       </c>
       <c r="M4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="1">
-        <v>23.26</v>
+        <v>23.2</v>
       </c>
       <c r="C5" s="1">
-        <v>-20.350000000000001</v>
+        <v>-22.8</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>23.75</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="3">
         <v>23.875</v>
       </c>
       <c r="K5">
         <f xml:space="preserve"> E5 - ABS(B5)</f>
-        <v>0.48999999999999844</v>
+        <v>0.55000000000000071</v>
       </c>
       <c r="L5">
         <f xml:space="preserve"> F5 - ABS(C5)</f>
-        <v>3.5249999999999986</v>
+        <v>1.0749999999999993</v>
       </c>
       <c r="M5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -713,18 +728,18 @@
       <c r="F8" s="1">
         <v>23.375</v>
       </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+    </row>
+    <row r="9" spans="1:13">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -737,7 +752,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -745,86 +760,98 @@
       <c r="F11" s="1"/>
       <c r="K11">
         <f>AVERAGE(K2:K5)</f>
-        <v>-0.22874999999999979</v>
+        <v>-5.6249999999999467E-2</v>
       </c>
       <c r="L11">
         <f>AVERAGE(L2:L5)</f>
-        <v>3.2524999999999986</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
       <c r="K13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13">
       <c r="K14">
         <f>K2-$K$11</f>
-        <v>4.8750000000000071E-2</v>
+        <v>-0.34374999999999911</v>
       </c>
       <c r="L14">
         <f>L2-$L$11</f>
-        <v>-0.18750000000000089</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+        <v>-0.35000000000000142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="2">
+        <f>47.5 - ABS(47)</f>
+        <v>0.5</v>
+      </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
       <c r="K15">
         <f>K3-$K$11</f>
-        <v>0.19374999999999964</v>
+        <v>0.28125000000000089</v>
       </c>
       <c r="L15">
         <f>L3-$L$11</f>
-        <v>-0.15749999999999975</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+        <v>-0.64999999999999858</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="8">
+        <f>47.625 - ABS(-49.1)</f>
+        <v>-1.4750000000000014</v>
+      </c>
+      <c r="H16">
+        <f>K2 +0.27875</f>
+        <v>-0.12124999999999858</v>
+      </c>
       <c r="K16">
         <f>K4-$K$11</f>
-        <v>-0.96124999999999794</v>
+        <v>-0.54375000000000195</v>
       </c>
       <c r="L16">
         <f>L4-$L$11</f>
-        <v>7.2500000000000675E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+        <v>0.30000000000000071</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="K17">
         <f>K5-$K$11</f>
-        <v>0.71874999999999822</v>
+        <v>0.60625000000000018</v>
       </c>
       <c r="L17">
         <f>L5-$L$11</f>
-        <v>0.27249999999999996</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+        <v>0.69999999999999929</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="O20">
         <f>K40-K11</f>
-        <v>0.24125000000000085</v>
+        <v>6.2499999999996447E-3</v>
       </c>
       <c r="P20">
         <f>L11-L40</f>
-        <v>-0.89750000000000085</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+        <v>0.32500000000000018</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="K28" t="s">
         <v>4</v>
       </c>
@@ -835,151 +862,157 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16">
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
       <c r="H29">
         <f>3/8</f>
         <v>0.375</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16">
       <c r="A30" t="s">
         <v>15</v>
       </c>
       <c r="B30" s="1">
-        <v>-23.34</v>
+        <v>-23.4</v>
       </c>
       <c r="C30" s="1">
-        <v>43.9</v>
+        <v>-47.5</v>
       </c>
       <c r="D30" s="1"/>
-      <c r="E30" s="2">
+      <c r="E30" s="3">
         <v>23.875</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="3">
         <v>47.625</v>
       </c>
       <c r="K30">
         <f xml:space="preserve"> E30 - ABS(B30)</f>
-        <v>0.53500000000000014</v>
+        <v>0.47500000000000142</v>
       </c>
       <c r="L30">
         <f xml:space="preserve"> F30 - ABS(C30)</f>
-        <v>3.7250000000000014</v>
+        <v>0.125</v>
       </c>
       <c r="M30">
         <f t="shared" ref="M30:M33" si="2" xml:space="preserve"> G30 - ABS(D30)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16">
       <c r="A31" t="s">
         <v>16</v>
       </c>
       <c r="B31" s="1">
-        <v>-47.48</v>
+        <v>-47.6</v>
       </c>
       <c r="C31" s="1">
-        <v>-44.45</v>
+        <v>-47.7</v>
       </c>
       <c r="D31" s="1"/>
-      <c r="E31" s="2">
+      <c r="E31" s="3">
         <v>47.625</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31" s="3">
         <v>47.625</v>
       </c>
       <c r="K31">
         <f xml:space="preserve"> E31 - ABS(B31)</f>
-        <v>0.14500000000000313</v>
+        <v>2.4999999999998579E-2</v>
       </c>
       <c r="L31">
         <f xml:space="preserve"> F31 - ABS(C31)</f>
-        <v>3.1749999999999972</v>
+        <v>-7.5000000000002842E-2</v>
       </c>
       <c r="M31">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16">
       <c r="A32" t="s">
         <v>17</v>
       </c>
       <c r="B32" s="1">
-        <v>-24.44</v>
+        <v>-24.2</v>
       </c>
       <c r="C32" s="1">
-        <v>-18.46</v>
+        <v>-23.2</v>
       </c>
       <c r="D32" s="1"/>
-      <c r="E32" s="2">
+      <c r="E32" s="3">
         <v>23.875</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32" s="3">
         <v>23.375</v>
       </c>
       <c r="K32">
         <f xml:space="preserve"> E32 - ABS(B32)</f>
-        <v>-0.56500000000000128</v>
+        <v>-0.32499999999999929</v>
       </c>
       <c r="L32">
         <f xml:space="preserve"> F32 - ABS(C32)</f>
-        <v>4.9149999999999991</v>
+        <v>0.17500000000000071</v>
       </c>
       <c r="M32">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13">
       <c r="A33" t="s">
         <v>18</v>
       </c>
       <c r="B33" s="1">
-        <v>-47.69</v>
+        <v>-48</v>
       </c>
       <c r="C33" s="1">
-        <v>-18.59</v>
+        <v>-23.4</v>
       </c>
       <c r="D33" s="1"/>
-      <c r="E33" s="2">
+      <c r="E33" s="3">
         <v>47.625</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" s="3">
         <v>23.375</v>
       </c>
       <c r="K33">
         <f xml:space="preserve"> E33 - ABS(B33)</f>
-        <v>-6.4999999999997726E-2</v>
+        <v>-0.375</v>
       </c>
       <c r="L33">
         <f xml:space="preserve"> F33 - ABS(C33)</f>
-        <v>4.7850000000000001</v>
+        <v>-2.4999999999998579E-2</v>
       </c>
       <c r="M33">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="5"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13">
+      <c r="A34" s="6"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+    </row>
+    <row r="36" spans="1:13">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+    </row>
+    <row r="39" spans="1:13">
       <c r="K39" t="s">
         <v>13</v>
       </c>
@@ -987,58 +1020,70 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13">
       <c r="K40">
         <f>AVERAGE(K30:K33)</f>
-        <v>1.2500000000001066E-2</v>
+        <v>-4.9999999999999822E-2</v>
       </c>
       <c r="L40">
         <f>AVERAGE(L30:L33)</f>
-        <v>4.1499999999999995</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+        <v>4.9999999999999822E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
       <c r="K42">
         <f>K30-$K$40</f>
-        <v>0.52249999999999908</v>
+        <v>0.52500000000000124</v>
       </c>
       <c r="L42">
         <f>L30-$L$40</f>
-        <v>-0.42499999999999805</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+        <v>7.5000000000000178E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
       <c r="K43">
         <f>K31-$K$40</f>
-        <v>0.13250000000000206</v>
+        <v>7.4999999999998401E-2</v>
       </c>
       <c r="L43">
         <f>L31-$L$40</f>
-        <v>-0.97500000000000231</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+        <v>-0.12500000000000266</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
       <c r="K44">
         <f>K32-$K$40</f>
-        <v>-0.57750000000000234</v>
+        <v>-0.27499999999999947</v>
       </c>
       <c r="L44">
         <f>L32-$L$40</f>
-        <v>0.76499999999999968</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.12500000000000089</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
       <c r="K45">
         <f>K33-$K$40</f>
-        <v>-7.7499999999998792E-2</v>
+        <v>-0.32500000000000018</v>
       </c>
       <c r="L45">
         <f>L33-$L$40</f>
-        <v>0.63500000000000068</v>
+        <v>-7.4999999999998401E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{103934DF-1143-0D43-AC5C-F4EA14CA0981}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>